<commit_message>
Se actualizan los formularios de registro masivo
</commit_message>
<xml_diff>
--- a/public/DownloadExcels/Mercancias.xlsx
+++ b/public/DownloadExcels/Mercancias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Mario\Desktop\Ecopcion Definitivo\ecopFront\public\DownloadExcels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Reyes\OneDrive - Top Drive Group\Escritorio\CARLOS\FORMULARIOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1401CBD-80D1-484B-AB5A-CA0575DBBC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F80D72-BC4C-4640-A4A5-32EA2F3F2796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTARIO DE MERCANCIAS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
   <si>
     <t xml:space="preserve">INVENTARIO DE MERCANCIAS </t>
   </si>
@@ -507,6 +507,12 @@
     </r>
   </si>
   <si>
+    <t>GATO</t>
+  </si>
+  <si>
+    <t>PERRO</t>
+  </si>
+  <si>
     <t>Precio unitario de venta</t>
   </si>
 </sst>
@@ -913,24 +919,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -957,6 +945,24 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -992,9 +998,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1745118</xdr:colOff>
+      <xdr:colOff>1748928</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>398287</xdr:rowOff>
+      <xdr:rowOff>415432</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1230,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z689"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1254,22 +1260,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="57"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="51"/>
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
       <c r="Q1" s="18"/>
@@ -1284,22 +1290,22 @@
       <c r="Z1" s="18"/>
     </row>
     <row r="2" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="60"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="54"/>
       <c r="O2" s="18"/>
       <c r="P2" s="18"/>
       <c r="Q2" s="18"/>
@@ -1314,22 +1320,22 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="285" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="63"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="57"/>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
@@ -1361,7 +1367,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H4" s="31" t="s">
         <v>69</v>
@@ -1457,14 +1463,30 @@
       <c r="A6" s="44">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="47"/>
+      <c r="B6" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="46">
+        <v>100</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="58">
+        <v>1500</v>
+      </c>
+      <c r="F6" s="47">
+        <v>5</v>
+      </c>
+      <c r="G6" s="58">
+        <v>1900</v>
+      </c>
+      <c r="H6" s="61">
+        <v>45657</v>
+      </c>
+      <c r="I6" s="47" t="s">
+        <v>23</v>
+      </c>
       <c r="J6" s="47"/>
       <c r="K6" s="46"/>
       <c r="L6" s="47"/>
@@ -1487,14 +1509,30 @@
       <c r="A7" s="36">
         <v>2</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="47"/>
+      <c r="B7" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="46">
+        <v>5</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="58">
+        <v>5000</v>
+      </c>
+      <c r="F7" s="47">
+        <v>19</v>
+      </c>
+      <c r="G7" s="58">
+        <v>2500</v>
+      </c>
+      <c r="H7" s="61">
+        <v>45658</v>
+      </c>
+      <c r="I7" s="47" t="s">
+        <v>5</v>
+      </c>
       <c r="J7" s="47"/>
       <c r="K7" s="46"/>
       <c r="L7" s="47"/>
@@ -1517,13 +1555,13 @@
       <c r="A8" s="36">
         <v>3</v>
       </c>
-      <c r="B8" s="48"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="46"/>
       <c r="D8" s="47"/>
-      <c r="E8" s="49"/>
+      <c r="E8" s="58"/>
       <c r="F8" s="47"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="52"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="61"/>
       <c r="I8" s="47"/>
       <c r="J8" s="47"/>
       <c r="K8" s="46"/>
@@ -1550,10 +1588,10 @@
       <c r="B9" s="45"/>
       <c r="C9" s="46"/>
       <c r="D9" s="47"/>
-      <c r="E9" s="49"/>
+      <c r="E9" s="58"/>
       <c r="F9" s="47"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="52"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="61"/>
       <c r="I9" s="47"/>
       <c r="J9" s="47"/>
       <c r="K9" s="46"/>
@@ -1580,10 +1618,10 @@
       <c r="B10" s="48"/>
       <c r="C10" s="46"/>
       <c r="D10" s="47"/>
-      <c r="E10" s="49"/>
+      <c r="E10" s="58"/>
       <c r="F10" s="47"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="52"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="61"/>
       <c r="I10" s="47"/>
       <c r="J10" s="47"/>
       <c r="K10" s="46"/>
@@ -1610,10 +1648,10 @@
       <c r="B11" s="48"/>
       <c r="C11" s="46"/>
       <c r="D11" s="47"/>
-      <c r="E11" s="49"/>
+      <c r="E11" s="58"/>
       <c r="F11" s="47"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="52"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="61"/>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
       <c r="K11" s="46"/>
@@ -1640,10 +1678,10 @@
       <c r="B12" s="48"/>
       <c r="C12" s="46"/>
       <c r="D12" s="47"/>
-      <c r="E12" s="49"/>
+      <c r="E12" s="58"/>
       <c r="F12" s="47"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="52"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="61"/>
       <c r="I12" s="47"/>
       <c r="J12" s="47"/>
       <c r="K12" s="46"/>
@@ -1670,10 +1708,10 @@
       <c r="B13" s="48"/>
       <c r="C13" s="46"/>
       <c r="D13" s="47"/>
-      <c r="E13" s="49"/>
+      <c r="E13" s="58"/>
       <c r="F13" s="47"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="52"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="61"/>
       <c r="I13" s="47"/>
       <c r="J13" s="47"/>
       <c r="K13" s="46"/>
@@ -1700,10 +1738,10 @@
       <c r="B14" s="48"/>
       <c r="C14" s="46"/>
       <c r="D14" s="47"/>
-      <c r="E14" s="49"/>
+      <c r="E14" s="58"/>
       <c r="F14" s="47"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="52"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="61"/>
       <c r="I14" s="47"/>
       <c r="J14" s="47"/>
       <c r="K14" s="46"/>
@@ -1730,10 +1768,10 @@
       <c r="B15" s="48"/>
       <c r="C15" s="46"/>
       <c r="D15" s="47"/>
-      <c r="E15" s="49"/>
+      <c r="E15" s="58"/>
       <c r="F15" s="47"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="52"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="61"/>
       <c r="I15" s="47"/>
       <c r="J15" s="47"/>
       <c r="K15" s="46"/>
@@ -1760,10 +1798,10 @@
       <c r="B16" s="48"/>
       <c r="C16" s="46"/>
       <c r="D16" s="47"/>
-      <c r="E16" s="49"/>
+      <c r="E16" s="58"/>
       <c r="F16" s="47"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="52"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="61"/>
       <c r="I16" s="47"/>
       <c r="J16" s="47"/>
       <c r="K16" s="46"/>
@@ -1790,10 +1828,10 @@
       <c r="B17" s="48"/>
       <c r="C17" s="46"/>
       <c r="D17" s="47"/>
-      <c r="E17" s="49"/>
+      <c r="E17" s="58"/>
       <c r="F17" s="47"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="52"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="61"/>
       <c r="I17" s="47"/>
       <c r="J17" s="47"/>
       <c r="K17" s="46"/>
@@ -1820,10 +1858,10 @@
       <c r="B18" s="48"/>
       <c r="C18" s="46"/>
       <c r="D18" s="47"/>
-      <c r="E18" s="49"/>
+      <c r="E18" s="58"/>
       <c r="F18" s="47"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="52"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="61"/>
       <c r="I18" s="47"/>
       <c r="J18" s="47"/>
       <c r="K18" s="46"/>
@@ -1850,10 +1888,10 @@
       <c r="B19" s="48"/>
       <c r="C19" s="46"/>
       <c r="D19" s="47"/>
-      <c r="E19" s="49"/>
+      <c r="E19" s="58"/>
       <c r="F19" s="47"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="52"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="61"/>
       <c r="I19" s="47"/>
       <c r="J19" s="47"/>
       <c r="K19" s="46"/>
@@ -1880,10 +1918,10 @@
       <c r="B20" s="48"/>
       <c r="C20" s="46"/>
       <c r="D20" s="47"/>
-      <c r="E20" s="49"/>
+      <c r="E20" s="58"/>
       <c r="F20" s="47"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="52"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="61"/>
       <c r="I20" s="47"/>
       <c r="J20" s="47"/>
       <c r="K20" s="46"/>
@@ -1910,10 +1948,10 @@
       <c r="B21" s="48"/>
       <c r="C21" s="46"/>
       <c r="D21" s="47"/>
-      <c r="E21" s="49"/>
+      <c r="E21" s="58"/>
       <c r="F21" s="47"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="52"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="61"/>
       <c r="I21" s="47"/>
       <c r="J21" s="47"/>
       <c r="K21" s="46"/>
@@ -1940,10 +1978,10 @@
       <c r="B22" s="48"/>
       <c r="C22" s="46"/>
       <c r="D22" s="47"/>
-      <c r="E22" s="49"/>
+      <c r="E22" s="58"/>
       <c r="F22" s="47"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="52"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="61"/>
       <c r="I22" s="47"/>
       <c r="J22" s="47"/>
       <c r="K22" s="46"/>
@@ -1970,10 +2008,10 @@
       <c r="B23" s="48"/>
       <c r="C23" s="46"/>
       <c r="D23" s="47"/>
-      <c r="E23" s="49"/>
+      <c r="E23" s="58"/>
       <c r="F23" s="47"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="52"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="61"/>
       <c r="I23" s="47"/>
       <c r="J23" s="47"/>
       <c r="K23" s="46"/>
@@ -2000,10 +2038,10 @@
       <c r="B24" s="48"/>
       <c r="C24" s="46"/>
       <c r="D24" s="47"/>
-      <c r="E24" s="49"/>
+      <c r="E24" s="58"/>
       <c r="F24" s="47"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="52"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="61"/>
       <c r="I24" s="47"/>
       <c r="J24" s="47"/>
       <c r="K24" s="46"/>
@@ -2030,10 +2068,10 @@
       <c r="B25" s="48"/>
       <c r="C25" s="46"/>
       <c r="D25" s="47"/>
-      <c r="E25" s="49"/>
+      <c r="E25" s="58"/>
       <c r="F25" s="47"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="52"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="61"/>
       <c r="I25" s="47"/>
       <c r="J25" s="47"/>
       <c r="K25" s="46"/>
@@ -2060,10 +2098,10 @@
       <c r="B26" s="48"/>
       <c r="C26" s="46"/>
       <c r="D26" s="47"/>
-      <c r="E26" s="49"/>
+      <c r="E26" s="58"/>
       <c r="F26" s="47"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="52"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="61"/>
       <c r="I26" s="47"/>
       <c r="J26" s="47"/>
       <c r="K26" s="46"/>
@@ -2090,10 +2128,10 @@
       <c r="B27" s="48"/>
       <c r="C27" s="46"/>
       <c r="D27" s="47"/>
-      <c r="E27" s="49"/>
+      <c r="E27" s="58"/>
       <c r="F27" s="47"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="52"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="61"/>
       <c r="I27" s="47"/>
       <c r="J27" s="47"/>
       <c r="K27" s="46"/>
@@ -2120,10 +2158,10 @@
       <c r="B28" s="48"/>
       <c r="C28" s="46"/>
       <c r="D28" s="47"/>
-      <c r="E28" s="49"/>
+      <c r="E28" s="58"/>
       <c r="F28" s="47"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="52"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="61"/>
       <c r="I28" s="47"/>
       <c r="J28" s="47"/>
       <c r="K28" s="46"/>
@@ -2150,10 +2188,10 @@
       <c r="B29" s="48"/>
       <c r="C29" s="46"/>
       <c r="D29" s="47"/>
-      <c r="E29" s="49"/>
+      <c r="E29" s="58"/>
       <c r="F29" s="47"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="52"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="61"/>
       <c r="I29" s="47"/>
       <c r="J29" s="47"/>
       <c r="K29" s="46"/>
@@ -2180,10 +2218,10 @@
       <c r="B30" s="48"/>
       <c r="C30" s="46"/>
       <c r="D30" s="47"/>
-      <c r="E30" s="49"/>
+      <c r="E30" s="58"/>
       <c r="F30" s="47"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="52"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="61"/>
       <c r="I30" s="47"/>
       <c r="J30" s="47"/>
       <c r="K30" s="46"/>
@@ -2210,10 +2248,10 @@
       <c r="B31" s="48"/>
       <c r="C31" s="46"/>
       <c r="D31" s="47"/>
-      <c r="E31" s="49"/>
+      <c r="E31" s="58"/>
       <c r="F31" s="47"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="52"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="61"/>
       <c r="I31" s="47"/>
       <c r="J31" s="47"/>
       <c r="K31" s="46"/>
@@ -2240,10 +2278,10 @@
       <c r="B32" s="48"/>
       <c r="C32" s="46"/>
       <c r="D32" s="47"/>
-      <c r="E32" s="49"/>
+      <c r="E32" s="58"/>
       <c r="F32" s="47"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="52"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="61"/>
       <c r="I32" s="47"/>
       <c r="J32" s="47"/>
       <c r="K32" s="46"/>
@@ -2270,10 +2308,10 @@
       <c r="B33" s="48"/>
       <c r="C33" s="46"/>
       <c r="D33" s="47"/>
-      <c r="E33" s="49"/>
+      <c r="E33" s="58"/>
       <c r="F33" s="47"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="52"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="61"/>
       <c r="I33" s="47"/>
       <c r="J33" s="47"/>
       <c r="K33" s="46"/>
@@ -2300,10 +2338,10 @@
       <c r="B34" s="48"/>
       <c r="C34" s="46"/>
       <c r="D34" s="47"/>
-      <c r="E34" s="49"/>
+      <c r="E34" s="58"/>
       <c r="F34" s="47"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="52"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="61"/>
       <c r="I34" s="47"/>
       <c r="J34" s="47"/>
       <c r="K34" s="46"/>
@@ -2330,10 +2368,10 @@
       <c r="B35" s="48"/>
       <c r="C35" s="46"/>
       <c r="D35" s="47"/>
-      <c r="E35" s="49"/>
+      <c r="E35" s="58"/>
       <c r="F35" s="47"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="52"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="61"/>
       <c r="I35" s="47"/>
       <c r="J35" s="47"/>
       <c r="K35" s="46"/>
@@ -2360,10 +2398,10 @@
       <c r="B36" s="48"/>
       <c r="C36" s="46"/>
       <c r="D36" s="47"/>
-      <c r="E36" s="49"/>
+      <c r="E36" s="58"/>
       <c r="F36" s="47"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="52"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="61"/>
       <c r="I36" s="47"/>
       <c r="J36" s="47"/>
       <c r="K36" s="46"/>
@@ -2390,10 +2428,10 @@
       <c r="B37" s="48"/>
       <c r="C37" s="46"/>
       <c r="D37" s="47"/>
-      <c r="E37" s="49"/>
+      <c r="E37" s="58"/>
       <c r="F37" s="47"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="52"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="61"/>
       <c r="I37" s="47"/>
       <c r="J37" s="47"/>
       <c r="K37" s="46"/>
@@ -2420,10 +2458,10 @@
       <c r="B38" s="48"/>
       <c r="C38" s="46"/>
       <c r="D38" s="47"/>
-      <c r="E38" s="49"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="47"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="52"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="61"/>
       <c r="I38" s="47"/>
       <c r="J38" s="47"/>
       <c r="K38" s="46"/>
@@ -2450,10 +2488,10 @@
       <c r="B39" s="27"/>
       <c r="C39" s="28"/>
       <c r="D39" s="29"/>
-      <c r="E39" s="50"/>
+      <c r="E39" s="59"/>
       <c r="F39" s="47"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="53"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="62"/>
       <c r="I39" s="29"/>
       <c r="J39" s="29"/>
       <c r="K39" s="28"/>
@@ -2480,10 +2518,10 @@
       <c r="B40" s="12"/>
       <c r="C40" s="20"/>
       <c r="D40" s="21"/>
-      <c r="E40" s="51"/>
+      <c r="E40" s="60"/>
       <c r="F40" s="47"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="54"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="63"/>
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
       <c r="K40" s="20"/>
@@ -2510,10 +2548,10 @@
       <c r="B41" s="12"/>
       <c r="C41" s="20"/>
       <c r="D41" s="21"/>
-      <c r="E41" s="51"/>
+      <c r="E41" s="60"/>
       <c r="F41" s="47"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="54"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="63"/>
       <c r="I41" s="21"/>
       <c r="J41" s="21"/>
       <c r="K41" s="20"/>
@@ -2540,10 +2578,10 @@
       <c r="B42" s="12"/>
       <c r="C42" s="20"/>
       <c r="D42" s="21"/>
-      <c r="E42" s="51"/>
+      <c r="E42" s="60"/>
       <c r="F42" s="47"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="54"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="63"/>
       <c r="I42" s="21"/>
       <c r="J42" s="21"/>
       <c r="K42" s="20"/>
@@ -2570,10 +2608,10 @@
       <c r="B43" s="12"/>
       <c r="C43" s="20"/>
       <c r="D43" s="21"/>
-      <c r="E43" s="51"/>
+      <c r="E43" s="60"/>
       <c r="F43" s="47"/>
-      <c r="G43" s="51"/>
-      <c r="H43" s="54"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="63"/>
       <c r="I43" s="21"/>
       <c r="J43" s="21"/>
       <c r="K43" s="20"/>
@@ -2600,10 +2638,10 @@
       <c r="B44" s="12"/>
       <c r="C44" s="20"/>
       <c r="D44" s="21"/>
-      <c r="E44" s="51"/>
+      <c r="E44" s="60"/>
       <c r="F44" s="47"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="54"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="63"/>
       <c r="I44" s="21"/>
       <c r="J44" s="21"/>
       <c r="K44" s="20"/>
@@ -2630,10 +2668,10 @@
       <c r="B45" s="12"/>
       <c r="C45" s="20"/>
       <c r="D45" s="21"/>
-      <c r="E45" s="51"/>
+      <c r="E45" s="60"/>
       <c r="F45" s="47"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="54"/>
+      <c r="G45" s="60"/>
+      <c r="H45" s="63"/>
       <c r="I45" s="21"/>
       <c r="J45" s="21"/>
       <c r="K45" s="20"/>
@@ -2660,10 +2698,10 @@
       <c r="B46" s="12"/>
       <c r="C46" s="20"/>
       <c r="D46" s="21"/>
-      <c r="E46" s="51"/>
+      <c r="E46" s="60"/>
       <c r="F46" s="47"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="54"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="63"/>
       <c r="I46" s="21"/>
       <c r="J46" s="21"/>
       <c r="K46" s="20"/>
@@ -2690,10 +2728,10 @@
       <c r="B47" s="12"/>
       <c r="C47" s="20"/>
       <c r="D47" s="21"/>
-      <c r="E47" s="51"/>
+      <c r="E47" s="60"/>
       <c r="F47" s="47"/>
-      <c r="G47" s="51"/>
-      <c r="H47" s="54"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="63"/>
       <c r="I47" s="21"/>
       <c r="J47" s="21"/>
       <c r="K47" s="20"/>
@@ -2720,10 +2758,10 @@
       <c r="B48" s="12"/>
       <c r="C48" s="20"/>
       <c r="D48" s="21"/>
-      <c r="E48" s="51"/>
+      <c r="E48" s="60"/>
       <c r="F48" s="47"/>
-      <c r="G48" s="51"/>
-      <c r="H48" s="54"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="63"/>
       <c r="I48" s="21"/>
       <c r="J48" s="21"/>
       <c r="K48" s="20"/>
@@ -2750,10 +2788,10 @@
       <c r="B49" s="12"/>
       <c r="C49" s="20"/>
       <c r="D49" s="21"/>
-      <c r="E49" s="51"/>
+      <c r="E49" s="60"/>
       <c r="F49" s="47"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="54"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="63"/>
       <c r="I49" s="21"/>
       <c r="J49" s="21"/>
       <c r="K49" s="20"/>
@@ -2780,10 +2818,10 @@
       <c r="B50" s="12"/>
       <c r="C50" s="20"/>
       <c r="D50" s="21"/>
-      <c r="E50" s="51"/>
+      <c r="E50" s="60"/>
       <c r="F50" s="47"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="54"/>
+      <c r="G50" s="60"/>
+      <c r="H50" s="63"/>
       <c r="I50" s="21"/>
       <c r="J50" s="21"/>
       <c r="K50" s="20"/>
@@ -2810,10 +2848,10 @@
       <c r="B51" s="12"/>
       <c r="C51" s="20"/>
       <c r="D51" s="21"/>
-      <c r="E51" s="51"/>
+      <c r="E51" s="60"/>
       <c r="F51" s="47"/>
-      <c r="G51" s="51"/>
-      <c r="H51" s="54"/>
+      <c r="G51" s="60"/>
+      <c r="H51" s="63"/>
       <c r="I51" s="21"/>
       <c r="J51" s="21"/>
       <c r="K51" s="20"/>
@@ -2840,10 +2878,10 @@
       <c r="B52" s="12"/>
       <c r="C52" s="20"/>
       <c r="D52" s="21"/>
-      <c r="E52" s="51"/>
+      <c r="E52" s="60"/>
       <c r="F52" s="47"/>
-      <c r="G52" s="51"/>
-      <c r="H52" s="54"/>
+      <c r="G52" s="60"/>
+      <c r="H52" s="63"/>
       <c r="I52" s="21"/>
       <c r="J52" s="21"/>
       <c r="K52" s="20"/>
@@ -2870,10 +2908,10 @@
       <c r="B53" s="12"/>
       <c r="C53" s="20"/>
       <c r="D53" s="21"/>
-      <c r="E53" s="51"/>
+      <c r="E53" s="60"/>
       <c r="F53" s="47"/>
-      <c r="G53" s="51"/>
-      <c r="H53" s="54"/>
+      <c r="G53" s="60"/>
+      <c r="H53" s="63"/>
       <c r="I53" s="21"/>
       <c r="J53" s="21"/>
       <c r="K53" s="20"/>
@@ -2900,10 +2938,10 @@
       <c r="B54" s="12"/>
       <c r="C54" s="20"/>
       <c r="D54" s="21"/>
-      <c r="E54" s="51"/>
+      <c r="E54" s="60"/>
       <c r="F54" s="47"/>
-      <c r="G54" s="51"/>
-      <c r="H54" s="54"/>
+      <c r="G54" s="60"/>
+      <c r="H54" s="63"/>
       <c r="I54" s="21"/>
       <c r="J54" s="21"/>
       <c r="K54" s="20"/>
@@ -2930,10 +2968,10 @@
       <c r="B55" s="12"/>
       <c r="C55" s="20"/>
       <c r="D55" s="21"/>
-      <c r="E55" s="51"/>
+      <c r="E55" s="60"/>
       <c r="F55" s="47"/>
-      <c r="G55" s="51"/>
-      <c r="H55" s="54"/>
+      <c r="G55" s="60"/>
+      <c r="H55" s="63"/>
       <c r="I55" s="21"/>
       <c r="J55" s="21"/>
       <c r="K55" s="20"/>
@@ -2960,10 +2998,10 @@
       <c r="B56" s="12"/>
       <c r="C56" s="20"/>
       <c r="D56" s="21"/>
-      <c r="E56" s="51"/>
+      <c r="E56" s="60"/>
       <c r="F56" s="47"/>
-      <c r="G56" s="51"/>
-      <c r="H56" s="54"/>
+      <c r="G56" s="60"/>
+      <c r="H56" s="63"/>
       <c r="I56" s="21"/>
       <c r="J56" s="21"/>
       <c r="K56" s="20"/>
@@ -2990,10 +3028,10 @@
       <c r="B57" s="12"/>
       <c r="C57" s="20"/>
       <c r="D57" s="21"/>
-      <c r="E57" s="51"/>
+      <c r="E57" s="60"/>
       <c r="F57" s="47"/>
-      <c r="G57" s="51"/>
-      <c r="H57" s="54"/>
+      <c r="G57" s="60"/>
+      <c r="H57" s="63"/>
       <c r="I57" s="21"/>
       <c r="J57" s="21"/>
       <c r="K57" s="20"/>
@@ -3020,10 +3058,10 @@
       <c r="B58" s="12"/>
       <c r="C58" s="20"/>
       <c r="D58" s="21"/>
-      <c r="E58" s="51"/>
+      <c r="E58" s="60"/>
       <c r="F58" s="47"/>
-      <c r="G58" s="51"/>
-      <c r="H58" s="54"/>
+      <c r="G58" s="60"/>
+      <c r="H58" s="63"/>
       <c r="I58" s="21"/>
       <c r="J58" s="21"/>
       <c r="K58" s="20"/>
@@ -3050,10 +3088,10 @@
       <c r="B59" s="12"/>
       <c r="C59" s="20"/>
       <c r="D59" s="21"/>
-      <c r="E59" s="51"/>
+      <c r="E59" s="60"/>
       <c r="F59" s="47"/>
-      <c r="G59" s="51"/>
-      <c r="H59" s="54"/>
+      <c r="G59" s="60"/>
+      <c r="H59" s="63"/>
       <c r="I59" s="21"/>
       <c r="J59" s="21"/>
       <c r="K59" s="20"/>
@@ -3080,10 +3118,10 @@
       <c r="B60" s="12"/>
       <c r="C60" s="20"/>
       <c r="D60" s="21"/>
-      <c r="E60" s="51"/>
+      <c r="E60" s="60"/>
       <c r="F60" s="47"/>
-      <c r="G60" s="51"/>
-      <c r="H60" s="54"/>
+      <c r="G60" s="60"/>
+      <c r="H60" s="63"/>
       <c r="I60" s="21"/>
       <c r="J60" s="21"/>
       <c r="K60" s="20"/>
@@ -3110,10 +3148,10 @@
       <c r="B61" s="12"/>
       <c r="C61" s="20"/>
       <c r="D61" s="21"/>
-      <c r="E61" s="51"/>
+      <c r="E61" s="60"/>
       <c r="F61" s="47"/>
-      <c r="G61" s="51"/>
-      <c r="H61" s="54"/>
+      <c r="G61" s="60"/>
+      <c r="H61" s="63"/>
       <c r="I61" s="21"/>
       <c r="J61" s="21"/>
       <c r="K61" s="20"/>
@@ -3140,10 +3178,10 @@
       <c r="B62" s="12"/>
       <c r="C62" s="20"/>
       <c r="D62" s="21"/>
-      <c r="E62" s="51"/>
+      <c r="E62" s="60"/>
       <c r="F62" s="47"/>
-      <c r="G62" s="51"/>
-      <c r="H62" s="54"/>
+      <c r="G62" s="60"/>
+      <c r="H62" s="63"/>
       <c r="I62" s="21"/>
       <c r="J62" s="21"/>
       <c r="K62" s="20"/>
@@ -3170,10 +3208,10 @@
       <c r="B63" s="12"/>
       <c r="C63" s="20"/>
       <c r="D63" s="21"/>
-      <c r="E63" s="51"/>
+      <c r="E63" s="60"/>
       <c r="F63" s="47"/>
-      <c r="G63" s="51"/>
-      <c r="H63" s="54"/>
+      <c r="G63" s="60"/>
+      <c r="H63" s="63"/>
       <c r="I63" s="21"/>
       <c r="J63" s="21"/>
       <c r="K63" s="20"/>
@@ -3200,10 +3238,10 @@
       <c r="B64" s="12"/>
       <c r="C64" s="20"/>
       <c r="D64" s="21"/>
-      <c r="E64" s="51"/>
+      <c r="E64" s="60"/>
       <c r="F64" s="47"/>
-      <c r="G64" s="51"/>
-      <c r="H64" s="54"/>
+      <c r="G64" s="60"/>
+      <c r="H64" s="63"/>
       <c r="I64" s="21"/>
       <c r="J64" s="21"/>
       <c r="K64" s="20"/>
@@ -3230,10 +3268,10 @@
       <c r="B65" s="12"/>
       <c r="C65" s="20"/>
       <c r="D65" s="21"/>
-      <c r="E65" s="51"/>
+      <c r="E65" s="60"/>
       <c r="F65" s="47"/>
-      <c r="G65" s="51"/>
-      <c r="H65" s="54"/>
+      <c r="G65" s="60"/>
+      <c r="H65" s="63"/>
       <c r="I65" s="21"/>
       <c r="J65" s="21"/>
       <c r="K65" s="20"/>
@@ -3260,10 +3298,10 @@
       <c r="B66" s="12"/>
       <c r="C66" s="20"/>
       <c r="D66" s="21"/>
-      <c r="E66" s="51"/>
+      <c r="E66" s="60"/>
       <c r="F66" s="47"/>
-      <c r="G66" s="51"/>
-      <c r="H66" s="54"/>
+      <c r="G66" s="60"/>
+      <c r="H66" s="63"/>
       <c r="I66" s="21"/>
       <c r="J66" s="21"/>
       <c r="K66" s="20"/>
@@ -3290,10 +3328,10 @@
       <c r="B67" s="12"/>
       <c r="C67" s="20"/>
       <c r="D67" s="21"/>
-      <c r="E67" s="51"/>
+      <c r="E67" s="60"/>
       <c r="F67" s="47"/>
-      <c r="G67" s="51"/>
-      <c r="H67" s="54"/>
+      <c r="G67" s="60"/>
+      <c r="H67" s="63"/>
       <c r="I67" s="21"/>
       <c r="J67" s="21"/>
       <c r="K67" s="20"/>
@@ -3320,10 +3358,10 @@
       <c r="B68" s="12"/>
       <c r="C68" s="20"/>
       <c r="D68" s="21"/>
-      <c r="E68" s="51"/>
+      <c r="E68" s="60"/>
       <c r="F68" s="47"/>
-      <c r="G68" s="51"/>
-      <c r="H68" s="54"/>
+      <c r="G68" s="60"/>
+      <c r="H68" s="63"/>
       <c r="I68" s="21"/>
       <c r="J68" s="21"/>
       <c r="K68" s="20"/>
@@ -3350,10 +3388,10 @@
       <c r="B69" s="12"/>
       <c r="C69" s="20"/>
       <c r="D69" s="21"/>
-      <c r="E69" s="51"/>
+      <c r="E69" s="60"/>
       <c r="F69" s="47"/>
-      <c r="G69" s="51"/>
-      <c r="H69" s="54"/>
+      <c r="G69" s="60"/>
+      <c r="H69" s="63"/>
       <c r="I69" s="21"/>
       <c r="J69" s="21"/>
       <c r="K69" s="20"/>
@@ -3380,10 +3418,10 @@
       <c r="B70" s="12"/>
       <c r="C70" s="20"/>
       <c r="D70" s="21"/>
-      <c r="E70" s="51"/>
+      <c r="E70" s="60"/>
       <c r="F70" s="47"/>
-      <c r="G70" s="51"/>
-      <c r="H70" s="54"/>
+      <c r="G70" s="60"/>
+      <c r="H70" s="63"/>
       <c r="I70" s="21"/>
       <c r="J70" s="21"/>
       <c r="K70" s="20"/>
@@ -3410,10 +3448,10 @@
       <c r="B71" s="12"/>
       <c r="C71" s="20"/>
       <c r="D71" s="21"/>
-      <c r="E71" s="51"/>
+      <c r="E71" s="60"/>
       <c r="F71" s="47"/>
-      <c r="G71" s="51"/>
-      <c r="H71" s="54"/>
+      <c r="G71" s="60"/>
+      <c r="H71" s="63"/>
       <c r="I71" s="21"/>
       <c r="J71" s="21"/>
       <c r="K71" s="20"/>
@@ -3440,10 +3478,10 @@
       <c r="B72" s="12"/>
       <c r="C72" s="20"/>
       <c r="D72" s="21"/>
-      <c r="E72" s="51"/>
+      <c r="E72" s="60"/>
       <c r="F72" s="47"/>
-      <c r="G72" s="51"/>
-      <c r="H72" s="54"/>
+      <c r="G72" s="60"/>
+      <c r="H72" s="63"/>
       <c r="I72" s="21"/>
       <c r="J72" s="21"/>
       <c r="K72" s="20"/>
@@ -3470,10 +3508,10 @@
       <c r="B73" s="12"/>
       <c r="C73" s="20"/>
       <c r="D73" s="21"/>
-      <c r="E73" s="51"/>
+      <c r="E73" s="60"/>
       <c r="F73" s="47"/>
-      <c r="G73" s="51"/>
-      <c r="H73" s="54"/>
+      <c r="G73" s="60"/>
+      <c r="H73" s="63"/>
       <c r="I73" s="21"/>
       <c r="J73" s="21"/>
       <c r="K73" s="20"/>
@@ -3500,10 +3538,10 @@
       <c r="B74" s="12"/>
       <c r="C74" s="20"/>
       <c r="D74" s="21"/>
-      <c r="E74" s="51"/>
+      <c r="E74" s="60"/>
       <c r="F74" s="47"/>
-      <c r="G74" s="51"/>
-      <c r="H74" s="54"/>
+      <c r="G74" s="60"/>
+      <c r="H74" s="63"/>
       <c r="I74" s="21"/>
       <c r="J74" s="21"/>
       <c r="K74" s="20"/>
@@ -3530,10 +3568,10 @@
       <c r="B75" s="12"/>
       <c r="C75" s="20"/>
       <c r="D75" s="21"/>
-      <c r="E75" s="51"/>
+      <c r="E75" s="60"/>
       <c r="F75" s="47"/>
-      <c r="G75" s="51"/>
-      <c r="H75" s="54"/>
+      <c r="G75" s="60"/>
+      <c r="H75" s="63"/>
       <c r="I75" s="21"/>
       <c r="J75" s="21"/>
       <c r="K75" s="20"/>
@@ -3560,10 +3598,10 @@
       <c r="B76" s="12"/>
       <c r="C76" s="20"/>
       <c r="D76" s="21"/>
-      <c r="E76" s="51"/>
+      <c r="E76" s="60"/>
       <c r="F76" s="47"/>
-      <c r="G76" s="51"/>
-      <c r="H76" s="54"/>
+      <c r="G76" s="60"/>
+      <c r="H76" s="63"/>
       <c r="I76" s="21"/>
       <c r="J76" s="21"/>
       <c r="K76" s="20"/>
@@ -3590,10 +3628,10 @@
       <c r="B77" s="12"/>
       <c r="C77" s="20"/>
       <c r="D77" s="21"/>
-      <c r="E77" s="51"/>
+      <c r="E77" s="60"/>
       <c r="F77" s="47"/>
-      <c r="G77" s="51"/>
-      <c r="H77" s="54"/>
+      <c r="G77" s="60"/>
+      <c r="H77" s="63"/>
       <c r="I77" s="21"/>
       <c r="J77" s="21"/>
       <c r="K77" s="20"/>
@@ -3620,10 +3658,10 @@
       <c r="B78" s="12"/>
       <c r="C78" s="20"/>
       <c r="D78" s="21"/>
-      <c r="E78" s="51"/>
+      <c r="E78" s="60"/>
       <c r="F78" s="47"/>
-      <c r="G78" s="51"/>
-      <c r="H78" s="54"/>
+      <c r="G78" s="60"/>
+      <c r="H78" s="63"/>
       <c r="I78" s="21"/>
       <c r="J78" s="21"/>
       <c r="K78" s="20"/>
@@ -3650,10 +3688,10 @@
       <c r="B79" s="12"/>
       <c r="C79" s="20"/>
       <c r="D79" s="21"/>
-      <c r="E79" s="51"/>
+      <c r="E79" s="60"/>
       <c r="F79" s="47"/>
-      <c r="G79" s="51"/>
-      <c r="H79" s="54"/>
+      <c r="G79" s="60"/>
+      <c r="H79" s="63"/>
       <c r="I79" s="21"/>
       <c r="J79" s="21"/>
       <c r="K79" s="20"/>
@@ -3680,10 +3718,10 @@
       <c r="B80" s="12"/>
       <c r="C80" s="20"/>
       <c r="D80" s="21"/>
-      <c r="E80" s="51"/>
+      <c r="E80" s="60"/>
       <c r="F80" s="47"/>
-      <c r="G80" s="51"/>
-      <c r="H80" s="54"/>
+      <c r="G80" s="60"/>
+      <c r="H80" s="63"/>
       <c r="I80" s="21"/>
       <c r="J80" s="21"/>
       <c r="K80" s="20"/>
@@ -3710,10 +3748,10 @@
       <c r="B81" s="12"/>
       <c r="C81" s="20"/>
       <c r="D81" s="21"/>
-      <c r="E81" s="51"/>
+      <c r="E81" s="60"/>
       <c r="F81" s="47"/>
-      <c r="G81" s="51"/>
-      <c r="H81" s="54"/>
+      <c r="G81" s="60"/>
+      <c r="H81" s="63"/>
       <c r="I81" s="21"/>
       <c r="J81" s="21"/>
       <c r="K81" s="20"/>
@@ -3740,10 +3778,10 @@
       <c r="B82" s="12"/>
       <c r="C82" s="20"/>
       <c r="D82" s="21"/>
-      <c r="E82" s="51"/>
+      <c r="E82" s="60"/>
       <c r="F82" s="47"/>
-      <c r="G82" s="51"/>
-      <c r="H82" s="54"/>
+      <c r="G82" s="60"/>
+      <c r="H82" s="63"/>
       <c r="I82" s="21"/>
       <c r="J82" s="21"/>
       <c r="K82" s="20"/>
@@ -3770,10 +3808,10 @@
       <c r="B83" s="12"/>
       <c r="C83" s="20"/>
       <c r="D83" s="21"/>
-      <c r="E83" s="51"/>
+      <c r="E83" s="60"/>
       <c r="F83" s="47"/>
-      <c r="G83" s="51"/>
-      <c r="H83" s="54"/>
+      <c r="G83" s="60"/>
+      <c r="H83" s="63"/>
       <c r="I83" s="21"/>
       <c r="J83" s="21"/>
       <c r="K83" s="20"/>
@@ -3800,10 +3838,10 @@
       <c r="B84" s="12"/>
       <c r="C84" s="20"/>
       <c r="D84" s="21"/>
-      <c r="E84" s="51"/>
+      <c r="E84" s="60"/>
       <c r="F84" s="47"/>
-      <c r="G84" s="51"/>
-      <c r="H84" s="54"/>
+      <c r="G84" s="60"/>
+      <c r="H84" s="63"/>
       <c r="I84" s="21"/>
       <c r="J84" s="21"/>
       <c r="K84" s="20"/>
@@ -3830,10 +3868,10 @@
       <c r="B85" s="12"/>
       <c r="C85" s="20"/>
       <c r="D85" s="21"/>
-      <c r="E85" s="51"/>
+      <c r="E85" s="60"/>
       <c r="F85" s="47"/>
-      <c r="G85" s="51"/>
-      <c r="H85" s="54"/>
+      <c r="G85" s="60"/>
+      <c r="H85" s="63"/>
       <c r="I85" s="21"/>
       <c r="J85" s="21"/>
       <c r="K85" s="20"/>
@@ -3860,10 +3898,10 @@
       <c r="B86" s="12"/>
       <c r="C86" s="20"/>
       <c r="D86" s="21"/>
-      <c r="E86" s="51"/>
+      <c r="E86" s="60"/>
       <c r="F86" s="47"/>
-      <c r="G86" s="51"/>
-      <c r="H86" s="54"/>
+      <c r="G86" s="60"/>
+      <c r="H86" s="63"/>
       <c r="I86" s="21"/>
       <c r="J86" s="21"/>
       <c r="K86" s="20"/>
@@ -3890,10 +3928,10 @@
       <c r="B87" s="12"/>
       <c r="C87" s="20"/>
       <c r="D87" s="21"/>
-      <c r="E87" s="51"/>
+      <c r="E87" s="60"/>
       <c r="F87" s="47"/>
-      <c r="G87" s="51"/>
-      <c r="H87" s="54"/>
+      <c r="G87" s="60"/>
+      <c r="H87" s="63"/>
       <c r="I87" s="21"/>
       <c r="J87" s="21"/>
       <c r="K87" s="20"/>
@@ -3920,10 +3958,10 @@
       <c r="B88" s="12"/>
       <c r="C88" s="20"/>
       <c r="D88" s="21"/>
-      <c r="E88" s="51"/>
+      <c r="E88" s="60"/>
       <c r="F88" s="47"/>
-      <c r="G88" s="51"/>
-      <c r="H88" s="54"/>
+      <c r="G88" s="60"/>
+      <c r="H88" s="63"/>
       <c r="I88" s="21"/>
       <c r="J88" s="21"/>
       <c r="K88" s="20"/>
@@ -3950,10 +3988,10 @@
       <c r="B89" s="12"/>
       <c r="C89" s="20"/>
       <c r="D89" s="21"/>
-      <c r="E89" s="51"/>
+      <c r="E89" s="60"/>
       <c r="F89" s="47"/>
-      <c r="G89" s="51"/>
-      <c r="H89" s="54"/>
+      <c r="G89" s="60"/>
+      <c r="H89" s="63"/>
       <c r="I89" s="21"/>
       <c r="J89" s="21"/>
       <c r="K89" s="20"/>
@@ -3980,10 +4018,10 @@
       <c r="B90" s="12"/>
       <c r="C90" s="20"/>
       <c r="D90" s="21"/>
-      <c r="E90" s="51"/>
+      <c r="E90" s="60"/>
       <c r="F90" s="47"/>
-      <c r="G90" s="51"/>
-      <c r="H90" s="54"/>
+      <c r="G90" s="60"/>
+      <c r="H90" s="63"/>
       <c r="I90" s="21"/>
       <c r="J90" s="21"/>
       <c r="K90" s="20"/>
@@ -4010,10 +4048,10 @@
       <c r="B91" s="12"/>
       <c r="C91" s="20"/>
       <c r="D91" s="21"/>
-      <c r="E91" s="51"/>
+      <c r="E91" s="60"/>
       <c r="F91" s="47"/>
-      <c r="G91" s="51"/>
-      <c r="H91" s="54"/>
+      <c r="G91" s="60"/>
+      <c r="H91" s="63"/>
       <c r="I91" s="21"/>
       <c r="J91" s="21"/>
       <c r="K91" s="20"/>
@@ -4040,10 +4078,10 @@
       <c r="B92" s="12"/>
       <c r="C92" s="20"/>
       <c r="D92" s="21"/>
-      <c r="E92" s="51"/>
+      <c r="E92" s="60"/>
       <c r="F92" s="47"/>
-      <c r="G92" s="51"/>
-      <c r="H92" s="54"/>
+      <c r="G92" s="60"/>
+      <c r="H92" s="63"/>
       <c r="I92" s="21"/>
       <c r="J92" s="21"/>
       <c r="K92" s="20"/>
@@ -4070,10 +4108,10 @@
       <c r="B93" s="12"/>
       <c r="C93" s="20"/>
       <c r="D93" s="21"/>
-      <c r="E93" s="51"/>
+      <c r="E93" s="60"/>
       <c r="F93" s="47"/>
-      <c r="G93" s="51"/>
-      <c r="H93" s="54"/>
+      <c r="G93" s="60"/>
+      <c r="H93" s="63"/>
       <c r="I93" s="21"/>
       <c r="J93" s="21"/>
       <c r="K93" s="20"/>
@@ -4100,10 +4138,10 @@
       <c r="B94" s="12"/>
       <c r="C94" s="20"/>
       <c r="D94" s="21"/>
-      <c r="E94" s="51"/>
+      <c r="E94" s="60"/>
       <c r="F94" s="47"/>
-      <c r="G94" s="51"/>
-      <c r="H94" s="54"/>
+      <c r="G94" s="60"/>
+      <c r="H94" s="63"/>
       <c r="I94" s="21"/>
       <c r="J94" s="21"/>
       <c r="K94" s="20"/>
@@ -4130,10 +4168,10 @@
       <c r="B95" s="12"/>
       <c r="C95" s="20"/>
       <c r="D95" s="21"/>
-      <c r="E95" s="51"/>
+      <c r="E95" s="60"/>
       <c r="F95" s="47"/>
-      <c r="G95" s="51"/>
-      <c r="H95" s="54"/>
+      <c r="G95" s="60"/>
+      <c r="H95" s="63"/>
       <c r="I95" s="21"/>
       <c r="J95" s="21"/>
       <c r="K95" s="20"/>
@@ -4160,10 +4198,10 @@
       <c r="B96" s="12"/>
       <c r="C96" s="20"/>
       <c r="D96" s="21"/>
-      <c r="E96" s="51"/>
+      <c r="E96" s="60"/>
       <c r="F96" s="47"/>
-      <c r="G96" s="51"/>
-      <c r="H96" s="54"/>
+      <c r="G96" s="60"/>
+      <c r="H96" s="63"/>
       <c r="I96" s="21"/>
       <c r="J96" s="21"/>
       <c r="K96" s="20"/>
@@ -4190,10 +4228,10 @@
       <c r="B97" s="12"/>
       <c r="C97" s="20"/>
       <c r="D97" s="21"/>
-      <c r="E97" s="51"/>
+      <c r="E97" s="60"/>
       <c r="F97" s="47"/>
-      <c r="G97" s="51"/>
-      <c r="H97" s="54"/>
+      <c r="G97" s="60"/>
+      <c r="H97" s="63"/>
       <c r="I97" s="21"/>
       <c r="J97" s="21"/>
       <c r="K97" s="20"/>
@@ -4220,10 +4258,10 @@
       <c r="B98" s="12"/>
       <c r="C98" s="20"/>
       <c r="D98" s="21"/>
-      <c r="E98" s="51"/>
+      <c r="E98" s="60"/>
       <c r="F98" s="47"/>
-      <c r="G98" s="51"/>
-      <c r="H98" s="54"/>
+      <c r="G98" s="60"/>
+      <c r="H98" s="63"/>
       <c r="I98" s="21"/>
       <c r="J98" s="21"/>
       <c r="K98" s="20"/>
@@ -4250,10 +4288,10 @@
       <c r="B99" s="12"/>
       <c r="C99" s="20"/>
       <c r="D99" s="21"/>
-      <c r="E99" s="51"/>
+      <c r="E99" s="60"/>
       <c r="F99" s="47"/>
-      <c r="G99" s="51"/>
-      <c r="H99" s="54"/>
+      <c r="G99" s="60"/>
+      <c r="H99" s="63"/>
       <c r="I99" s="21"/>
       <c r="J99" s="21"/>
       <c r="K99" s="20"/>
@@ -4280,10 +4318,10 @@
       <c r="B100" s="12"/>
       <c r="C100" s="20"/>
       <c r="D100" s="21"/>
-      <c r="E100" s="51"/>
+      <c r="E100" s="60"/>
       <c r="F100" s="47"/>
-      <c r="G100" s="51"/>
-      <c r="H100" s="54"/>
+      <c r="G100" s="60"/>
+      <c r="H100" s="63"/>
       <c r="I100" s="21"/>
       <c r="J100" s="21"/>
       <c r="K100" s="20"/>
@@ -4310,10 +4348,10 @@
       <c r="B101" s="12"/>
       <c r="C101" s="20"/>
       <c r="D101" s="21"/>
-      <c r="E101" s="51"/>
+      <c r="E101" s="60"/>
       <c r="F101" s="47"/>
-      <c r="G101" s="51"/>
-      <c r="H101" s="54"/>
+      <c r="G101" s="60"/>
+      <c r="H101" s="63"/>
       <c r="I101" s="21"/>
       <c r="J101" s="21"/>
       <c r="K101" s="20"/>
@@ -4340,10 +4378,10 @@
       <c r="B102" s="12"/>
       <c r="C102" s="20"/>
       <c r="D102" s="21"/>
-      <c r="E102" s="51"/>
+      <c r="E102" s="60"/>
       <c r="F102" s="47"/>
-      <c r="G102" s="51"/>
-      <c r="H102" s="54"/>
+      <c r="G102" s="60"/>
+      <c r="H102" s="63"/>
       <c r="I102" s="21"/>
       <c r="J102" s="21"/>
       <c r="K102" s="20"/>
@@ -4370,10 +4408,10 @@
       <c r="B103" s="12"/>
       <c r="C103" s="20"/>
       <c r="D103" s="21"/>
-      <c r="E103" s="51"/>
+      <c r="E103" s="60"/>
       <c r="F103" s="47"/>
-      <c r="G103" s="51"/>
-      <c r="H103" s="54"/>
+      <c r="G103" s="60"/>
+      <c r="H103" s="63"/>
       <c r="I103" s="21"/>
       <c r="J103" s="21"/>
       <c r="K103" s="20"/>
@@ -4400,10 +4438,10 @@
       <c r="B104" s="12"/>
       <c r="C104" s="20"/>
       <c r="D104" s="21"/>
-      <c r="E104" s="51"/>
+      <c r="E104" s="60"/>
       <c r="F104" s="47"/>
-      <c r="G104" s="51"/>
-      <c r="H104" s="54"/>
+      <c r="G104" s="60"/>
+      <c r="H104" s="63"/>
       <c r="I104" s="21"/>
       <c r="J104" s="21"/>
       <c r="K104" s="20"/>
@@ -4430,10 +4468,10 @@
       <c r="B105" s="12"/>
       <c r="C105" s="20"/>
       <c r="D105" s="21"/>
-      <c r="E105" s="51"/>
+      <c r="E105" s="60"/>
       <c r="F105" s="47"/>
-      <c r="G105" s="51"/>
-      <c r="H105" s="54"/>
+      <c r="G105" s="60"/>
+      <c r="H105" s="63"/>
       <c r="I105" s="21"/>
       <c r="J105" s="21"/>
       <c r="K105" s="20"/>
@@ -4460,10 +4498,10 @@
       <c r="B106" s="12"/>
       <c r="C106" s="20"/>
       <c r="D106" s="21"/>
-      <c r="E106" s="51"/>
+      <c r="E106" s="60"/>
       <c r="F106" s="47"/>
-      <c r="G106" s="51"/>
-      <c r="H106" s="54"/>
+      <c r="G106" s="60"/>
+      <c r="H106" s="63"/>
       <c r="I106" s="21"/>
       <c r="J106" s="21"/>
       <c r="K106" s="20"/>
@@ -4490,10 +4528,10 @@
       <c r="B107" s="12"/>
       <c r="C107" s="20"/>
       <c r="D107" s="21"/>
-      <c r="E107" s="51"/>
+      <c r="E107" s="60"/>
       <c r="F107" s="47"/>
-      <c r="G107" s="51"/>
-      <c r="H107" s="54"/>
+      <c r="G107" s="60"/>
+      <c r="H107" s="63"/>
       <c r="I107" s="21"/>
       <c r="J107" s="21"/>
       <c r="K107" s="20"/>
@@ -4520,10 +4558,10 @@
       <c r="B108" s="12"/>
       <c r="C108" s="20"/>
       <c r="D108" s="21"/>
-      <c r="E108" s="51"/>
+      <c r="E108" s="60"/>
       <c r="F108" s="47"/>
-      <c r="G108" s="51"/>
-      <c r="H108" s="54"/>
+      <c r="G108" s="60"/>
+      <c r="H108" s="63"/>
       <c r="I108" s="21"/>
       <c r="J108" s="21"/>
       <c r="K108" s="20"/>
@@ -4550,10 +4588,10 @@
       <c r="B109" s="12"/>
       <c r="C109" s="20"/>
       <c r="D109" s="21"/>
-      <c r="E109" s="51"/>
+      <c r="E109" s="60"/>
       <c r="F109" s="47"/>
-      <c r="G109" s="51"/>
-      <c r="H109" s="54"/>
+      <c r="G109" s="60"/>
+      <c r="H109" s="63"/>
       <c r="I109" s="21"/>
       <c r="J109" s="21"/>
       <c r="K109" s="20"/>
@@ -4580,10 +4618,10 @@
       <c r="B110" s="12"/>
       <c r="C110" s="20"/>
       <c r="D110" s="21"/>
-      <c r="E110" s="51"/>
+      <c r="E110" s="60"/>
       <c r="F110" s="47"/>
-      <c r="G110" s="51"/>
-      <c r="H110" s="54"/>
+      <c r="G110" s="60"/>
+      <c r="H110" s="63"/>
       <c r="I110" s="21"/>
       <c r="J110" s="21"/>
       <c r="K110" s="20"/>
@@ -4610,10 +4648,10 @@
       <c r="B111" s="12"/>
       <c r="C111" s="20"/>
       <c r="D111" s="21"/>
-      <c r="E111" s="51"/>
+      <c r="E111" s="60"/>
       <c r="F111" s="47"/>
-      <c r="G111" s="51"/>
-      <c r="H111" s="54"/>
+      <c r="G111" s="60"/>
+      <c r="H111" s="63"/>
       <c r="I111" s="21"/>
       <c r="J111" s="21"/>
       <c r="K111" s="20"/>
@@ -4640,10 +4678,10 @@
       <c r="B112" s="12"/>
       <c r="C112" s="20"/>
       <c r="D112" s="21"/>
-      <c r="E112" s="51"/>
+      <c r="E112" s="60"/>
       <c r="F112" s="47"/>
-      <c r="G112" s="51"/>
-      <c r="H112" s="54"/>
+      <c r="G112" s="60"/>
+      <c r="H112" s="63"/>
       <c r="I112" s="21"/>
       <c r="J112" s="21"/>
       <c r="K112" s="20"/>
@@ -4670,10 +4708,10 @@
       <c r="B113" s="12"/>
       <c r="C113" s="20"/>
       <c r="D113" s="21"/>
-      <c r="E113" s="51"/>
+      <c r="E113" s="60"/>
       <c r="F113" s="47"/>
-      <c r="G113" s="51"/>
-      <c r="H113" s="54"/>
+      <c r="G113" s="60"/>
+      <c r="H113" s="63"/>
       <c r="I113" s="21"/>
       <c r="J113" s="21"/>
       <c r="K113" s="20"/>
@@ -4700,10 +4738,10 @@
       <c r="B114" s="12"/>
       <c r="C114" s="20"/>
       <c r="D114" s="21"/>
-      <c r="E114" s="51"/>
+      <c r="E114" s="60"/>
       <c r="F114" s="47"/>
-      <c r="G114" s="51"/>
-      <c r="H114" s="54"/>
+      <c r="G114" s="60"/>
+      <c r="H114" s="63"/>
       <c r="I114" s="21"/>
       <c r="J114" s="21"/>
       <c r="K114" s="20"/>
@@ -4730,10 +4768,10 @@
       <c r="B115" s="12"/>
       <c r="C115" s="20"/>
       <c r="D115" s="21"/>
-      <c r="E115" s="51"/>
+      <c r="E115" s="60"/>
       <c r="F115" s="47"/>
-      <c r="G115" s="51"/>
-      <c r="H115" s="54"/>
+      <c r="G115" s="60"/>
+      <c r="H115" s="63"/>
       <c r="I115" s="21"/>
       <c r="J115" s="21"/>
       <c r="K115" s="20"/>
@@ -4760,10 +4798,10 @@
       <c r="B116" s="12"/>
       <c r="C116" s="20"/>
       <c r="D116" s="21"/>
-      <c r="E116" s="51"/>
+      <c r="E116" s="60"/>
       <c r="F116" s="47"/>
-      <c r="G116" s="51"/>
-      <c r="H116" s="54"/>
+      <c r="G116" s="60"/>
+      <c r="H116" s="63"/>
       <c r="I116" s="21"/>
       <c r="J116" s="21"/>
       <c r="K116" s="20"/>
@@ -4790,10 +4828,10 @@
       <c r="B117" s="12"/>
       <c r="C117" s="20"/>
       <c r="D117" s="21"/>
-      <c r="E117" s="51"/>
+      <c r="E117" s="60"/>
       <c r="F117" s="47"/>
-      <c r="G117" s="51"/>
-      <c r="H117" s="54"/>
+      <c r="G117" s="60"/>
+      <c r="H117" s="63"/>
       <c r="I117" s="21"/>
       <c r="J117" s="21"/>
       <c r="K117" s="20"/>
@@ -4820,10 +4858,10 @@
       <c r="B118" s="12"/>
       <c r="C118" s="20"/>
       <c r="D118" s="21"/>
-      <c r="E118" s="51"/>
+      <c r="E118" s="60"/>
       <c r="F118" s="47"/>
-      <c r="G118" s="51"/>
-      <c r="H118" s="54"/>
+      <c r="G118" s="60"/>
+      <c r="H118" s="63"/>
       <c r="I118" s="21"/>
       <c r="J118" s="21"/>
       <c r="K118" s="20"/>
@@ -4850,10 +4888,10 @@
       <c r="B119" s="12"/>
       <c r="C119" s="20"/>
       <c r="D119" s="21"/>
-      <c r="E119" s="51"/>
+      <c r="E119" s="60"/>
       <c r="F119" s="47"/>
-      <c r="G119" s="51"/>
-      <c r="H119" s="54"/>
+      <c r="G119" s="60"/>
+      <c r="H119" s="63"/>
       <c r="I119" s="21"/>
       <c r="J119" s="21"/>
       <c r="K119" s="20"/>
@@ -4880,10 +4918,10 @@
       <c r="B120" s="12"/>
       <c r="C120" s="20"/>
       <c r="D120" s="21"/>
-      <c r="E120" s="51"/>
+      <c r="E120" s="60"/>
       <c r="F120" s="47"/>
-      <c r="G120" s="51"/>
-      <c r="H120" s="54"/>
+      <c r="G120" s="60"/>
+      <c r="H120" s="63"/>
       <c r="I120" s="21"/>
       <c r="J120" s="21"/>
       <c r="K120" s="20"/>
@@ -4910,10 +4948,10 @@
       <c r="B121" s="12"/>
       <c r="C121" s="20"/>
       <c r="D121" s="21"/>
-      <c r="E121" s="51"/>
+      <c r="E121" s="60"/>
       <c r="F121" s="47"/>
-      <c r="G121" s="51"/>
-      <c r="H121" s="54"/>
+      <c r="G121" s="60"/>
+      <c r="H121" s="63"/>
       <c r="I121" s="21"/>
       <c r="J121" s="21"/>
       <c r="K121" s="20"/>
@@ -4940,10 +4978,10 @@
       <c r="B122" s="12"/>
       <c r="C122" s="20"/>
       <c r="D122" s="21"/>
-      <c r="E122" s="51"/>
+      <c r="E122" s="60"/>
       <c r="F122" s="47"/>
-      <c r="G122" s="51"/>
-      <c r="H122" s="54"/>
+      <c r="G122" s="60"/>
+      <c r="H122" s="63"/>
       <c r="I122" s="21"/>
       <c r="J122" s="21"/>
       <c r="K122" s="20"/>
@@ -4970,10 +5008,10 @@
       <c r="B123" s="12"/>
       <c r="C123" s="20"/>
       <c r="D123" s="21"/>
-      <c r="E123" s="51"/>
+      <c r="E123" s="60"/>
       <c r="F123" s="47"/>
-      <c r="G123" s="51"/>
-      <c r="H123" s="54"/>
+      <c r="G123" s="60"/>
+      <c r="H123" s="63"/>
       <c r="I123" s="21"/>
       <c r="J123" s="21"/>
       <c r="K123" s="20"/>
@@ -5000,10 +5038,10 @@
       <c r="B124" s="12"/>
       <c r="C124" s="20"/>
       <c r="D124" s="21"/>
-      <c r="E124" s="51"/>
+      <c r="E124" s="60"/>
       <c r="F124" s="47"/>
-      <c r="G124" s="51"/>
-      <c r="H124" s="54"/>
+      <c r="G124" s="60"/>
+      <c r="H124" s="63"/>
       <c r="I124" s="21"/>
       <c r="J124" s="21"/>
       <c r="K124" s="20"/>
@@ -5030,10 +5068,10 @@
       <c r="B125" s="12"/>
       <c r="C125" s="20"/>
       <c r="D125" s="21"/>
-      <c r="E125" s="51"/>
+      <c r="E125" s="60"/>
       <c r="F125" s="47"/>
-      <c r="G125" s="51"/>
-      <c r="H125" s="54"/>
+      <c r="G125" s="60"/>
+      <c r="H125" s="63"/>
       <c r="I125" s="21"/>
       <c r="J125" s="21"/>
       <c r="K125" s="20"/>
@@ -5060,10 +5098,10 @@
       <c r="B126" s="12"/>
       <c r="C126" s="20"/>
       <c r="D126" s="21"/>
-      <c r="E126" s="51"/>
+      <c r="E126" s="60"/>
       <c r="F126" s="47"/>
-      <c r="G126" s="51"/>
-      <c r="H126" s="54"/>
+      <c r="G126" s="60"/>
+      <c r="H126" s="63"/>
       <c r="I126" s="21"/>
       <c r="J126" s="21"/>
       <c r="K126" s="20"/>
@@ -5090,10 +5128,10 @@
       <c r="B127" s="12"/>
       <c r="C127" s="20"/>
       <c r="D127" s="21"/>
-      <c r="E127" s="51"/>
+      <c r="E127" s="60"/>
       <c r="F127" s="47"/>
-      <c r="G127" s="51"/>
-      <c r="H127" s="54"/>
+      <c r="G127" s="60"/>
+      <c r="H127" s="63"/>
       <c r="I127" s="21"/>
       <c r="J127" s="21"/>
       <c r="K127" s="20"/>
@@ -5120,10 +5158,10 @@
       <c r="B128" s="12"/>
       <c r="C128" s="20"/>
       <c r="D128" s="21"/>
-      <c r="E128" s="51"/>
+      <c r="E128" s="60"/>
       <c r="F128" s="47"/>
-      <c r="G128" s="51"/>
-      <c r="H128" s="54"/>
+      <c r="G128" s="60"/>
+      <c r="H128" s="63"/>
       <c r="I128" s="21"/>
       <c r="J128" s="21"/>
       <c r="K128" s="20"/>
@@ -5150,10 +5188,10 @@
       <c r="B129" s="12"/>
       <c r="C129" s="20"/>
       <c r="D129" s="21"/>
-      <c r="E129" s="51"/>
+      <c r="E129" s="60"/>
       <c r="F129" s="47"/>
-      <c r="G129" s="51"/>
-      <c r="H129" s="54"/>
+      <c r="G129" s="60"/>
+      <c r="H129" s="63"/>
       <c r="I129" s="21"/>
       <c r="J129" s="21"/>
       <c r="K129" s="20"/>
@@ -5180,10 +5218,10 @@
       <c r="B130" s="12"/>
       <c r="C130" s="20"/>
       <c r="D130" s="21"/>
-      <c r="E130" s="51"/>
+      <c r="E130" s="60"/>
       <c r="F130" s="47"/>
-      <c r="G130" s="51"/>
-      <c r="H130" s="54"/>
+      <c r="G130" s="60"/>
+      <c r="H130" s="63"/>
       <c r="I130" s="21"/>
       <c r="J130" s="21"/>
       <c r="K130" s="20"/>
@@ -5210,10 +5248,10 @@
       <c r="B131" s="12"/>
       <c r="C131" s="20"/>
       <c r="D131" s="21"/>
-      <c r="E131" s="51"/>
+      <c r="E131" s="60"/>
       <c r="F131" s="47"/>
-      <c r="G131" s="51"/>
-      <c r="H131" s="54"/>
+      <c r="G131" s="60"/>
+      <c r="H131" s="63"/>
       <c r="I131" s="21"/>
       <c r="J131" s="21"/>
       <c r="K131" s="20"/>
@@ -5240,10 +5278,10 @@
       <c r="B132" s="12"/>
       <c r="C132" s="20"/>
       <c r="D132" s="21"/>
-      <c r="E132" s="51"/>
+      <c r="E132" s="60"/>
       <c r="F132" s="47"/>
-      <c r="G132" s="51"/>
-      <c r="H132" s="54"/>
+      <c r="G132" s="60"/>
+      <c r="H132" s="63"/>
       <c r="I132" s="21"/>
       <c r="J132" s="21"/>
       <c r="K132" s="20"/>
@@ -5270,10 +5308,10 @@
       <c r="B133" s="12"/>
       <c r="C133" s="20"/>
       <c r="D133" s="21"/>
-      <c r="E133" s="51"/>
+      <c r="E133" s="60"/>
       <c r="F133" s="47"/>
-      <c r="G133" s="51"/>
-      <c r="H133" s="54"/>
+      <c r="G133" s="60"/>
+      <c r="H133" s="63"/>
       <c r="I133" s="21"/>
       <c r="J133" s="21"/>
       <c r="K133" s="20"/>
@@ -5300,10 +5338,10 @@
       <c r="B134" s="12"/>
       <c r="C134" s="20"/>
       <c r="D134" s="21"/>
-      <c r="E134" s="51"/>
+      <c r="E134" s="60"/>
       <c r="F134" s="47"/>
-      <c r="G134" s="51"/>
-      <c r="H134" s="54"/>
+      <c r="G134" s="60"/>
+      <c r="H134" s="63"/>
       <c r="I134" s="21"/>
       <c r="J134" s="21"/>
       <c r="K134" s="20"/>
@@ -5330,10 +5368,10 @@
       <c r="B135" s="12"/>
       <c r="C135" s="20"/>
       <c r="D135" s="21"/>
-      <c r="E135" s="51"/>
+      <c r="E135" s="60"/>
       <c r="F135" s="47"/>
-      <c r="G135" s="51"/>
-      <c r="H135" s="54"/>
+      <c r="G135" s="60"/>
+      <c r="H135" s="63"/>
       <c r="I135" s="21"/>
       <c r="J135" s="21"/>
       <c r="K135" s="20"/>
@@ -5360,10 +5398,10 @@
       <c r="B136" s="12"/>
       <c r="C136" s="20"/>
       <c r="D136" s="21"/>
-      <c r="E136" s="51"/>
+      <c r="E136" s="60"/>
       <c r="F136" s="47"/>
-      <c r="G136" s="51"/>
-      <c r="H136" s="54"/>
+      <c r="G136" s="60"/>
+      <c r="H136" s="63"/>
       <c r="I136" s="21"/>
       <c r="J136" s="21"/>
       <c r="K136" s="20"/>
@@ -5390,10 +5428,10 @@
       <c r="B137" s="12"/>
       <c r="C137" s="20"/>
       <c r="D137" s="21"/>
-      <c r="E137" s="51"/>
+      <c r="E137" s="60"/>
       <c r="F137" s="47"/>
-      <c r="G137" s="51"/>
-      <c r="H137" s="54"/>
+      <c r="G137" s="60"/>
+      <c r="H137" s="63"/>
       <c r="I137" s="21"/>
       <c r="J137" s="21"/>
       <c r="K137" s="20"/>
@@ -5420,10 +5458,10 @@
       <c r="B138" s="12"/>
       <c r="C138" s="20"/>
       <c r="D138" s="21"/>
-      <c r="E138" s="51"/>
+      <c r="E138" s="60"/>
       <c r="F138" s="47"/>
-      <c r="G138" s="51"/>
-      <c r="H138" s="54"/>
+      <c r="G138" s="60"/>
+      <c r="H138" s="63"/>
       <c r="I138" s="21"/>
       <c r="J138" s="21"/>
       <c r="K138" s="20"/>
@@ -5450,10 +5488,10 @@
       <c r="B139" s="12"/>
       <c r="C139" s="20"/>
       <c r="D139" s="21"/>
-      <c r="E139" s="51"/>
+      <c r="E139" s="60"/>
       <c r="F139" s="47"/>
-      <c r="G139" s="51"/>
-      <c r="H139" s="54"/>
+      <c r="G139" s="60"/>
+      <c r="H139" s="63"/>
       <c r="I139" s="21"/>
       <c r="J139" s="21"/>
       <c r="K139" s="20"/>
@@ -5480,10 +5518,10 @@
       <c r="B140" s="12"/>
       <c r="C140" s="20"/>
       <c r="D140" s="21"/>
-      <c r="E140" s="51"/>
+      <c r="E140" s="60"/>
       <c r="F140" s="47"/>
-      <c r="G140" s="51"/>
-      <c r="H140" s="54"/>
+      <c r="G140" s="60"/>
+      <c r="H140" s="63"/>
       <c r="I140" s="21"/>
       <c r="J140" s="21"/>
       <c r="K140" s="20"/>
@@ -5510,10 +5548,10 @@
       <c r="B141" s="12"/>
       <c r="C141" s="20"/>
       <c r="D141" s="21"/>
-      <c r="E141" s="51"/>
+      <c r="E141" s="60"/>
       <c r="F141" s="47"/>
-      <c r="G141" s="51"/>
-      <c r="H141" s="54"/>
+      <c r="G141" s="60"/>
+      <c r="H141" s="63"/>
       <c r="I141" s="21"/>
       <c r="J141" s="21"/>
       <c r="K141" s="20"/>
@@ -5540,10 +5578,10 @@
       <c r="B142" s="12"/>
       <c r="C142" s="20"/>
       <c r="D142" s="21"/>
-      <c r="E142" s="51"/>
+      <c r="E142" s="60"/>
       <c r="F142" s="47"/>
-      <c r="G142" s="51"/>
-      <c r="H142" s="54"/>
+      <c r="G142" s="60"/>
+      <c r="H142" s="63"/>
       <c r="I142" s="21"/>
       <c r="J142" s="21"/>
       <c r="K142" s="20"/>
@@ -5570,10 +5608,10 @@
       <c r="B143" s="12"/>
       <c r="C143" s="20"/>
       <c r="D143" s="21"/>
-      <c r="E143" s="51"/>
+      <c r="E143" s="60"/>
       <c r="F143" s="47"/>
-      <c r="G143" s="51"/>
-      <c r="H143" s="54"/>
+      <c r="G143" s="60"/>
+      <c r="H143" s="63"/>
       <c r="I143" s="21"/>
       <c r="J143" s="21"/>
       <c r="K143" s="20"/>
@@ -5600,10 +5638,10 @@
       <c r="B144" s="12"/>
       <c r="C144" s="20"/>
       <c r="D144" s="21"/>
-      <c r="E144" s="51"/>
+      <c r="E144" s="60"/>
       <c r="F144" s="47"/>
-      <c r="G144" s="51"/>
-      <c r="H144" s="54"/>
+      <c r="G144" s="60"/>
+      <c r="H144" s="63"/>
       <c r="I144" s="21"/>
       <c r="J144" s="21"/>
       <c r="K144" s="20"/>
@@ -5630,10 +5668,10 @@
       <c r="B145" s="12"/>
       <c r="C145" s="20"/>
       <c r="D145" s="21"/>
-      <c r="E145" s="51"/>
+      <c r="E145" s="60"/>
       <c r="F145" s="47"/>
-      <c r="G145" s="51"/>
-      <c r="H145" s="54"/>
+      <c r="G145" s="60"/>
+      <c r="H145" s="63"/>
       <c r="I145" s="21"/>
       <c r="J145" s="21"/>
       <c r="K145" s="20"/>
@@ -5660,10 +5698,10 @@
       <c r="B146" s="12"/>
       <c r="C146" s="20"/>
       <c r="D146" s="21"/>
-      <c r="E146" s="51"/>
+      <c r="E146" s="60"/>
       <c r="F146" s="47"/>
-      <c r="G146" s="51"/>
-      <c r="H146" s="54"/>
+      <c r="G146" s="60"/>
+      <c r="H146" s="63"/>
       <c r="I146" s="21"/>
       <c r="J146" s="21"/>
       <c r="K146" s="20"/>
@@ -5690,10 +5728,10 @@
       <c r="B147" s="12"/>
       <c r="C147" s="20"/>
       <c r="D147" s="21"/>
-      <c r="E147" s="51"/>
+      <c r="E147" s="60"/>
       <c r="F147" s="47"/>
-      <c r="G147" s="51"/>
-      <c r="H147" s="54"/>
+      <c r="G147" s="60"/>
+      <c r="H147" s="63"/>
       <c r="I147" s="21"/>
       <c r="J147" s="21"/>
       <c r="K147" s="20"/>
@@ -5720,10 +5758,10 @@
       <c r="B148" s="12"/>
       <c r="C148" s="20"/>
       <c r="D148" s="21"/>
-      <c r="E148" s="51"/>
+      <c r="E148" s="60"/>
       <c r="F148" s="47"/>
-      <c r="G148" s="51"/>
-      <c r="H148" s="54"/>
+      <c r="G148" s="60"/>
+      <c r="H148" s="63"/>
       <c r="I148" s="21"/>
       <c r="J148" s="21"/>
       <c r="K148" s="20"/>
@@ -5750,10 +5788,10 @@
       <c r="B149" s="12"/>
       <c r="C149" s="20"/>
       <c r="D149" s="21"/>
-      <c r="E149" s="51"/>
+      <c r="E149" s="60"/>
       <c r="F149" s="47"/>
-      <c r="G149" s="51"/>
-      <c r="H149" s="54"/>
+      <c r="G149" s="60"/>
+      <c r="H149" s="63"/>
       <c r="I149" s="21"/>
       <c r="J149" s="21"/>
       <c r="K149" s="20"/>
@@ -5780,10 +5818,10 @@
       <c r="B150" s="12"/>
       <c r="C150" s="20"/>
       <c r="D150" s="21"/>
-      <c r="E150" s="51"/>
+      <c r="E150" s="60"/>
       <c r="F150" s="47"/>
-      <c r="G150" s="51"/>
-      <c r="H150" s="54"/>
+      <c r="G150" s="60"/>
+      <c r="H150" s="63"/>
       <c r="I150" s="21"/>
       <c r="J150" s="21"/>
       <c r="K150" s="20"/>
@@ -5810,10 +5848,10 @@
       <c r="B151" s="12"/>
       <c r="C151" s="20"/>
       <c r="D151" s="21"/>
-      <c r="E151" s="51"/>
+      <c r="E151" s="60"/>
       <c r="F151" s="47"/>
-      <c r="G151" s="51"/>
-      <c r="H151" s="54"/>
+      <c r="G151" s="60"/>
+      <c r="H151" s="63"/>
       <c r="I151" s="21"/>
       <c r="J151" s="21"/>
       <c r="K151" s="20"/>
@@ -5840,10 +5878,10 @@
       <c r="B152" s="12"/>
       <c r="C152" s="20"/>
       <c r="D152" s="21"/>
-      <c r="E152" s="51"/>
+      <c r="E152" s="60"/>
       <c r="F152" s="47"/>
-      <c r="G152" s="51"/>
-      <c r="H152" s="54"/>
+      <c r="G152" s="60"/>
+      <c r="H152" s="63"/>
       <c r="I152" s="21"/>
       <c r="J152" s="21"/>
       <c r="K152" s="20"/>
@@ -5870,10 +5908,10 @@
       <c r="B153" s="12"/>
       <c r="C153" s="20"/>
       <c r="D153" s="21"/>
-      <c r="E153" s="51"/>
+      <c r="E153" s="60"/>
       <c r="F153" s="47"/>
-      <c r="G153" s="51"/>
-      <c r="H153" s="54"/>
+      <c r="G153" s="60"/>
+      <c r="H153" s="63"/>
       <c r="I153" s="21"/>
       <c r="J153" s="21"/>
       <c r="K153" s="20"/>
@@ -5900,10 +5938,10 @@
       <c r="B154" s="12"/>
       <c r="C154" s="20"/>
       <c r="D154" s="21"/>
-      <c r="E154" s="51"/>
+      <c r="E154" s="60"/>
       <c r="F154" s="47"/>
-      <c r="G154" s="51"/>
-      <c r="H154" s="54"/>
+      <c r="G154" s="60"/>
+      <c r="H154" s="63"/>
       <c r="I154" s="21"/>
       <c r="J154" s="21"/>
       <c r="K154" s="20"/>
@@ -5930,10 +5968,10 @@
       <c r="B155" s="12"/>
       <c r="C155" s="20"/>
       <c r="D155" s="21"/>
-      <c r="E155" s="51"/>
+      <c r="E155" s="60"/>
       <c r="F155" s="47"/>
-      <c r="G155" s="51"/>
-      <c r="H155" s="54"/>
+      <c r="G155" s="60"/>
+      <c r="H155" s="63"/>
       <c r="I155" s="21"/>
       <c r="J155" s="21"/>
       <c r="K155" s="20"/>
@@ -5960,10 +5998,10 @@
       <c r="B156" s="12"/>
       <c r="C156" s="20"/>
       <c r="D156" s="21"/>
-      <c r="E156" s="51"/>
+      <c r="E156" s="60"/>
       <c r="F156" s="47"/>
-      <c r="G156" s="51"/>
-      <c r="H156" s="54"/>
+      <c r="G156" s="60"/>
+      <c r="H156" s="63"/>
       <c r="I156" s="21"/>
       <c r="J156" s="21"/>
       <c r="K156" s="20"/>
@@ -5990,10 +6028,10 @@
       <c r="B157" s="12"/>
       <c r="C157" s="20"/>
       <c r="D157" s="21"/>
-      <c r="E157" s="51"/>
+      <c r="E157" s="60"/>
       <c r="F157" s="47"/>
-      <c r="G157" s="51"/>
-      <c r="H157" s="54"/>
+      <c r="G157" s="60"/>
+      <c r="H157" s="63"/>
       <c r="I157" s="21"/>
       <c r="J157" s="21"/>
       <c r="K157" s="20"/>
@@ -6020,10 +6058,10 @@
       <c r="B158" s="12"/>
       <c r="C158" s="20"/>
       <c r="D158" s="21"/>
-      <c r="E158" s="51"/>
+      <c r="E158" s="60"/>
       <c r="F158" s="47"/>
-      <c r="G158" s="51"/>
-      <c r="H158" s="54"/>
+      <c r="G158" s="60"/>
+      <c r="H158" s="63"/>
       <c r="I158" s="21"/>
       <c r="J158" s="21"/>
       <c r="K158" s="20"/>
@@ -6050,10 +6088,10 @@
       <c r="B159" s="12"/>
       <c r="C159" s="20"/>
       <c r="D159" s="21"/>
-      <c r="E159" s="51"/>
+      <c r="E159" s="60"/>
       <c r="F159" s="47"/>
-      <c r="G159" s="51"/>
-      <c r="H159" s="54"/>
+      <c r="G159" s="60"/>
+      <c r="H159" s="63"/>
       <c r="I159" s="21"/>
       <c r="J159" s="21"/>
       <c r="K159" s="20"/>
@@ -6080,10 +6118,10 @@
       <c r="B160" s="12"/>
       <c r="C160" s="20"/>
       <c r="D160" s="21"/>
-      <c r="E160" s="51"/>
+      <c r="E160" s="60"/>
       <c r="F160" s="47"/>
-      <c r="G160" s="51"/>
-      <c r="H160" s="54"/>
+      <c r="G160" s="60"/>
+      <c r="H160" s="63"/>
       <c r="I160" s="21"/>
       <c r="J160" s="21"/>
       <c r="K160" s="20"/>
@@ -6110,10 +6148,10 @@
       <c r="B161" s="12"/>
       <c r="C161" s="20"/>
       <c r="D161" s="21"/>
-      <c r="E161" s="51"/>
+      <c r="E161" s="60"/>
       <c r="F161" s="47"/>
-      <c r="G161" s="51"/>
-      <c r="H161" s="54"/>
+      <c r="G161" s="60"/>
+      <c r="H161" s="63"/>
       <c r="I161" s="21"/>
       <c r="J161" s="21"/>
       <c r="K161" s="20"/>
@@ -6140,10 +6178,10 @@
       <c r="B162" s="12"/>
       <c r="C162" s="20"/>
       <c r="D162" s="21"/>
-      <c r="E162" s="51"/>
+      <c r="E162" s="60"/>
       <c r="F162" s="47"/>
-      <c r="G162" s="51"/>
-      <c r="H162" s="54"/>
+      <c r="G162" s="60"/>
+      <c r="H162" s="63"/>
       <c r="I162" s="21"/>
       <c r="J162" s="21"/>
       <c r="K162" s="20"/>
@@ -6170,10 +6208,10 @@
       <c r="B163" s="12"/>
       <c r="C163" s="20"/>
       <c r="D163" s="21"/>
-      <c r="E163" s="51"/>
+      <c r="E163" s="60"/>
       <c r="F163" s="47"/>
-      <c r="G163" s="51"/>
-      <c r="H163" s="54"/>
+      <c r="G163" s="60"/>
+      <c r="H163" s="63"/>
       <c r="I163" s="21"/>
       <c r="J163" s="21"/>
       <c r="K163" s="20"/>
@@ -6200,10 +6238,10 @@
       <c r="B164" s="12"/>
       <c r="C164" s="20"/>
       <c r="D164" s="21"/>
-      <c r="E164" s="51"/>
+      <c r="E164" s="60"/>
       <c r="F164" s="47"/>
-      <c r="G164" s="51"/>
-      <c r="H164" s="54"/>
+      <c r="G164" s="60"/>
+      <c r="H164" s="63"/>
       <c r="I164" s="21"/>
       <c r="J164" s="21"/>
       <c r="K164" s="20"/>
@@ -6230,10 +6268,10 @@
       <c r="B165" s="12"/>
       <c r="C165" s="20"/>
       <c r="D165" s="21"/>
-      <c r="E165" s="51"/>
+      <c r="E165" s="60"/>
       <c r="F165" s="47"/>
-      <c r="G165" s="51"/>
-      <c r="H165" s="54"/>
+      <c r="G165" s="60"/>
+      <c r="H165" s="63"/>
       <c r="I165" s="21"/>
       <c r="J165" s="21"/>
       <c r="K165" s="20"/>
@@ -6260,10 +6298,10 @@
       <c r="B166" s="12"/>
       <c r="C166" s="20"/>
       <c r="D166" s="21"/>
-      <c r="E166" s="51"/>
+      <c r="E166" s="60"/>
       <c r="F166" s="47"/>
-      <c r="G166" s="51"/>
-      <c r="H166" s="54"/>
+      <c r="G166" s="60"/>
+      <c r="H166" s="63"/>
       <c r="I166" s="21"/>
       <c r="J166" s="21"/>
       <c r="K166" s="20"/>
@@ -6290,10 +6328,10 @@
       <c r="B167" s="12"/>
       <c r="C167" s="20"/>
       <c r="D167" s="21"/>
-      <c r="E167" s="51"/>
+      <c r="E167" s="60"/>
       <c r="F167" s="47"/>
-      <c r="G167" s="51"/>
-      <c r="H167" s="54"/>
+      <c r="G167" s="60"/>
+      <c r="H167" s="63"/>
       <c r="I167" s="21"/>
       <c r="J167" s="21"/>
       <c r="K167" s="20"/>
@@ -6320,10 +6358,10 @@
       <c r="B168" s="12"/>
       <c r="C168" s="20"/>
       <c r="D168" s="21"/>
-      <c r="E168" s="51"/>
+      <c r="E168" s="60"/>
       <c r="F168" s="47"/>
-      <c r="G168" s="51"/>
-      <c r="H168" s="54"/>
+      <c r="G168" s="60"/>
+      <c r="H168" s="63"/>
       <c r="I168" s="21"/>
       <c r="J168" s="21"/>
       <c r="K168" s="20"/>
@@ -6350,10 +6388,10 @@
       <c r="B169" s="12"/>
       <c r="C169" s="20"/>
       <c r="D169" s="21"/>
-      <c r="E169" s="51"/>
+      <c r="E169" s="60"/>
       <c r="F169" s="47"/>
-      <c r="G169" s="51"/>
-      <c r="H169" s="54"/>
+      <c r="G169" s="60"/>
+      <c r="H169" s="63"/>
       <c r="I169" s="21"/>
       <c r="J169" s="21"/>
       <c r="K169" s="20"/>
@@ -6380,10 +6418,10 @@
       <c r="B170" s="12"/>
       <c r="C170" s="20"/>
       <c r="D170" s="21"/>
-      <c r="E170" s="51"/>
+      <c r="E170" s="60"/>
       <c r="F170" s="47"/>
-      <c r="G170" s="51"/>
-      <c r="H170" s="54"/>
+      <c r="G170" s="60"/>
+      <c r="H170" s="63"/>
       <c r="I170" s="21"/>
       <c r="J170" s="21"/>
       <c r="K170" s="20"/>
@@ -6410,10 +6448,10 @@
       <c r="B171" s="12"/>
       <c r="C171" s="20"/>
       <c r="D171" s="21"/>
-      <c r="E171" s="51"/>
+      <c r="E171" s="60"/>
       <c r="F171" s="47"/>
-      <c r="G171" s="51"/>
-      <c r="H171" s="54"/>
+      <c r="G171" s="60"/>
+      <c r="H171" s="63"/>
       <c r="I171" s="21"/>
       <c r="J171" s="21"/>
       <c r="K171" s="20"/>
@@ -6440,10 +6478,10 @@
       <c r="B172" s="12"/>
       <c r="C172" s="20"/>
       <c r="D172" s="21"/>
-      <c r="E172" s="51"/>
+      <c r="E172" s="60"/>
       <c r="F172" s="47"/>
-      <c r="G172" s="51"/>
-      <c r="H172" s="54"/>
+      <c r="G172" s="60"/>
+      <c r="H172" s="63"/>
       <c r="I172" s="21"/>
       <c r="J172" s="21"/>
       <c r="K172" s="20"/>
@@ -6470,10 +6508,10 @@
       <c r="B173" s="12"/>
       <c r="C173" s="20"/>
       <c r="D173" s="21"/>
-      <c r="E173" s="51"/>
+      <c r="E173" s="60"/>
       <c r="F173" s="47"/>
-      <c r="G173" s="51"/>
-      <c r="H173" s="54"/>
+      <c r="G173" s="60"/>
+      <c r="H173" s="63"/>
       <c r="I173" s="21"/>
       <c r="J173" s="21"/>
       <c r="K173" s="20"/>
@@ -6500,10 +6538,10 @@
       <c r="B174" s="12"/>
       <c r="C174" s="20"/>
       <c r="D174" s="21"/>
-      <c r="E174" s="51"/>
+      <c r="E174" s="60"/>
       <c r="F174" s="47"/>
-      <c r="G174" s="51"/>
-      <c r="H174" s="54"/>
+      <c r="G174" s="60"/>
+      <c r="H174" s="63"/>
       <c r="I174" s="21"/>
       <c r="J174" s="21"/>
       <c r="K174" s="20"/>
@@ -6530,10 +6568,10 @@
       <c r="B175" s="12"/>
       <c r="C175" s="20"/>
       <c r="D175" s="21"/>
-      <c r="E175" s="51"/>
+      <c r="E175" s="60"/>
       <c r="F175" s="47"/>
-      <c r="G175" s="51"/>
-      <c r="H175" s="54"/>
+      <c r="G175" s="60"/>
+      <c r="H175" s="63"/>
       <c r="I175" s="21"/>
       <c r="J175" s="21"/>
       <c r="K175" s="20"/>
@@ -6560,10 +6598,10 @@
       <c r="B176" s="12"/>
       <c r="C176" s="20"/>
       <c r="D176" s="21"/>
-      <c r="E176" s="51"/>
+      <c r="E176" s="60"/>
       <c r="F176" s="47"/>
-      <c r="G176" s="51"/>
-      <c r="H176" s="54"/>
+      <c r="G176" s="60"/>
+      <c r="H176" s="63"/>
       <c r="I176" s="21"/>
       <c r="J176" s="21"/>
       <c r="K176" s="20"/>
@@ -6590,10 +6628,10 @@
       <c r="B177" s="12"/>
       <c r="C177" s="20"/>
       <c r="D177" s="21"/>
-      <c r="E177" s="51"/>
+      <c r="E177" s="60"/>
       <c r="F177" s="47"/>
-      <c r="G177" s="51"/>
-      <c r="H177" s="54"/>
+      <c r="G177" s="60"/>
+      <c r="H177" s="63"/>
       <c r="I177" s="21"/>
       <c r="J177" s="21"/>
       <c r="K177" s="20"/>
@@ -6620,10 +6658,10 @@
       <c r="B178" s="12"/>
       <c r="C178" s="20"/>
       <c r="D178" s="21"/>
-      <c r="E178" s="51"/>
+      <c r="E178" s="60"/>
       <c r="F178" s="47"/>
-      <c r="G178" s="51"/>
-      <c r="H178" s="54"/>
+      <c r="G178" s="60"/>
+      <c r="H178" s="63"/>
       <c r="I178" s="21"/>
       <c r="J178" s="21"/>
       <c r="K178" s="20"/>
@@ -6650,10 +6688,10 @@
       <c r="B179" s="12"/>
       <c r="C179" s="20"/>
       <c r="D179" s="21"/>
-      <c r="E179" s="51"/>
+      <c r="E179" s="60"/>
       <c r="F179" s="47"/>
-      <c r="G179" s="51"/>
-      <c r="H179" s="54"/>
+      <c r="G179" s="60"/>
+      <c r="H179" s="63"/>
       <c r="I179" s="21"/>
       <c r="J179" s="21"/>
       <c r="K179" s="20"/>
@@ -6680,10 +6718,10 @@
       <c r="B180" s="12"/>
       <c r="C180" s="20"/>
       <c r="D180" s="21"/>
-      <c r="E180" s="51"/>
+      <c r="E180" s="60"/>
       <c r="F180" s="47"/>
-      <c r="G180" s="51"/>
-      <c r="H180" s="54"/>
+      <c r="G180" s="60"/>
+      <c r="H180" s="63"/>
       <c r="I180" s="21"/>
       <c r="J180" s="21"/>
       <c r="K180" s="20"/>
@@ -6710,10 +6748,10 @@
       <c r="B181" s="12"/>
       <c r="C181" s="20"/>
       <c r="D181" s="21"/>
-      <c r="E181" s="51"/>
+      <c r="E181" s="60"/>
       <c r="F181" s="47"/>
-      <c r="G181" s="51"/>
-      <c r="H181" s="54"/>
+      <c r="G181" s="60"/>
+      <c r="H181" s="63"/>
       <c r="I181" s="21"/>
       <c r="J181" s="21"/>
       <c r="K181" s="20"/>
@@ -6740,10 +6778,10 @@
       <c r="B182" s="12"/>
       <c r="C182" s="20"/>
       <c r="D182" s="21"/>
-      <c r="E182" s="51"/>
+      <c r="E182" s="60"/>
       <c r="F182" s="47"/>
-      <c r="G182" s="51"/>
-      <c r="H182" s="54"/>
+      <c r="G182" s="60"/>
+      <c r="H182" s="63"/>
       <c r="I182" s="21"/>
       <c r="J182" s="21"/>
       <c r="K182" s="20"/>
@@ -6770,10 +6808,10 @@
       <c r="B183" s="12"/>
       <c r="C183" s="20"/>
       <c r="D183" s="21"/>
-      <c r="E183" s="51"/>
+      <c r="E183" s="60"/>
       <c r="F183" s="47"/>
-      <c r="G183" s="51"/>
-      <c r="H183" s="54"/>
+      <c r="G183" s="60"/>
+      <c r="H183" s="63"/>
       <c r="I183" s="21"/>
       <c r="J183" s="21"/>
       <c r="K183" s="20"/>
@@ -6800,10 +6838,10 @@
       <c r="B184" s="12"/>
       <c r="C184" s="20"/>
       <c r="D184" s="21"/>
-      <c r="E184" s="51"/>
+      <c r="E184" s="60"/>
       <c r="F184" s="47"/>
-      <c r="G184" s="51"/>
-      <c r="H184" s="54"/>
+      <c r="G184" s="60"/>
+      <c r="H184" s="63"/>
       <c r="I184" s="21"/>
       <c r="J184" s="21"/>
       <c r="K184" s="20"/>
@@ -6830,10 +6868,10 @@
       <c r="B185" s="12"/>
       <c r="C185" s="20"/>
       <c r="D185" s="21"/>
-      <c r="E185" s="51"/>
+      <c r="E185" s="60"/>
       <c r="F185" s="47"/>
-      <c r="G185" s="51"/>
-      <c r="H185" s="54"/>
+      <c r="G185" s="60"/>
+      <c r="H185" s="63"/>
       <c r="I185" s="21"/>
       <c r="J185" s="21"/>
       <c r="K185" s="20"/>
@@ -6860,10 +6898,10 @@
       <c r="B186" s="12"/>
       <c r="C186" s="20"/>
       <c r="D186" s="21"/>
-      <c r="E186" s="51"/>
+      <c r="E186" s="60"/>
       <c r="F186" s="47"/>
-      <c r="G186" s="51"/>
-      <c r="H186" s="54"/>
+      <c r="G186" s="60"/>
+      <c r="H186" s="63"/>
       <c r="I186" s="21"/>
       <c r="J186" s="21"/>
       <c r="K186" s="20"/>
@@ -6890,10 +6928,10 @@
       <c r="B187" s="12"/>
       <c r="C187" s="20"/>
       <c r="D187" s="21"/>
-      <c r="E187" s="51"/>
+      <c r="E187" s="60"/>
       <c r="F187" s="47"/>
-      <c r="G187" s="51"/>
-      <c r="H187" s="54"/>
+      <c r="G187" s="60"/>
+      <c r="H187" s="63"/>
       <c r="I187" s="21"/>
       <c r="J187" s="21"/>
       <c r="K187" s="20"/>
@@ -6920,10 +6958,10 @@
       <c r="B188" s="12"/>
       <c r="C188" s="20"/>
       <c r="D188" s="21"/>
-      <c r="E188" s="51"/>
+      <c r="E188" s="60"/>
       <c r="F188" s="47"/>
-      <c r="G188" s="51"/>
-      <c r="H188" s="54"/>
+      <c r="G188" s="60"/>
+      <c r="H188" s="63"/>
       <c r="I188" s="21"/>
       <c r="J188" s="21"/>
       <c r="K188" s="20"/>
@@ -6950,10 +6988,10 @@
       <c r="B189" s="12"/>
       <c r="C189" s="20"/>
       <c r="D189" s="21"/>
-      <c r="E189" s="51"/>
+      <c r="E189" s="60"/>
       <c r="F189" s="47"/>
-      <c r="G189" s="51"/>
-      <c r="H189" s="54"/>
+      <c r="G189" s="60"/>
+      <c r="H189" s="63"/>
       <c r="I189" s="21"/>
       <c r="J189" s="21"/>
       <c r="K189" s="20"/>
@@ -6980,10 +7018,10 @@
       <c r="B190" s="12"/>
       <c r="C190" s="20"/>
       <c r="D190" s="21"/>
-      <c r="E190" s="51"/>
+      <c r="E190" s="60"/>
       <c r="F190" s="47"/>
-      <c r="G190" s="51"/>
-      <c r="H190" s="54"/>
+      <c r="G190" s="60"/>
+      <c r="H190" s="63"/>
       <c r="I190" s="21"/>
       <c r="J190" s="21"/>
       <c r="K190" s="20"/>
@@ -7010,10 +7048,10 @@
       <c r="B191" s="12"/>
       <c r="C191" s="20"/>
       <c r="D191" s="21"/>
-      <c r="E191" s="51"/>
+      <c r="E191" s="60"/>
       <c r="F191" s="47"/>
-      <c r="G191" s="51"/>
-      <c r="H191" s="54"/>
+      <c r="G191" s="60"/>
+      <c r="H191" s="63"/>
       <c r="I191" s="21"/>
       <c r="J191" s="21"/>
       <c r="K191" s="20"/>
@@ -7040,10 +7078,10 @@
       <c r="B192" s="12"/>
       <c r="C192" s="20"/>
       <c r="D192" s="21"/>
-      <c r="E192" s="51"/>
+      <c r="E192" s="60"/>
       <c r="F192" s="47"/>
-      <c r="G192" s="51"/>
-      <c r="H192" s="54"/>
+      <c r="G192" s="60"/>
+      <c r="H192" s="63"/>
       <c r="I192" s="21"/>
       <c r="J192" s="21"/>
       <c r="K192" s="20"/>
@@ -7070,10 +7108,10 @@
       <c r="B193" s="12"/>
       <c r="C193" s="20"/>
       <c r="D193" s="21"/>
-      <c r="E193" s="51"/>
+      <c r="E193" s="60"/>
       <c r="F193" s="47"/>
-      <c r="G193" s="51"/>
-      <c r="H193" s="54"/>
+      <c r="G193" s="60"/>
+      <c r="H193" s="63"/>
       <c r="I193" s="21"/>
       <c r="J193" s="21"/>
       <c r="K193" s="20"/>
@@ -7100,10 +7138,10 @@
       <c r="B194" s="12"/>
       <c r="C194" s="20"/>
       <c r="D194" s="21"/>
-      <c r="E194" s="51"/>
+      <c r="E194" s="60"/>
       <c r="F194" s="47"/>
-      <c r="G194" s="51"/>
-      <c r="H194" s="54"/>
+      <c r="G194" s="60"/>
+      <c r="H194" s="63"/>
       <c r="I194" s="21"/>
       <c r="J194" s="21"/>
       <c r="K194" s="20"/>
@@ -7130,10 +7168,10 @@
       <c r="B195" s="12"/>
       <c r="C195" s="20"/>
       <c r="D195" s="21"/>
-      <c r="E195" s="51"/>
+      <c r="E195" s="60"/>
       <c r="F195" s="47"/>
-      <c r="G195" s="51"/>
-      <c r="H195" s="54"/>
+      <c r="G195" s="60"/>
+      <c r="H195" s="63"/>
       <c r="I195" s="21"/>
       <c r="J195" s="21"/>
       <c r="K195" s="20"/>
@@ -7160,10 +7198,10 @@
       <c r="B196" s="12"/>
       <c r="C196" s="20"/>
       <c r="D196" s="21"/>
-      <c r="E196" s="51"/>
+      <c r="E196" s="60"/>
       <c r="F196" s="47"/>
-      <c r="G196" s="51"/>
-      <c r="H196" s="54"/>
+      <c r="G196" s="60"/>
+      <c r="H196" s="63"/>
       <c r="I196" s="21"/>
       <c r="J196" s="21"/>
       <c r="K196" s="20"/>
@@ -7190,10 +7228,10 @@
       <c r="B197" s="12"/>
       <c r="C197" s="20"/>
       <c r="D197" s="21"/>
-      <c r="E197" s="51"/>
+      <c r="E197" s="60"/>
       <c r="F197" s="47"/>
-      <c r="G197" s="51"/>
-      <c r="H197" s="54"/>
+      <c r="G197" s="60"/>
+      <c r="H197" s="63"/>
       <c r="I197" s="21"/>
       <c r="J197" s="21"/>
       <c r="K197" s="20"/>
@@ -7220,10 +7258,10 @@
       <c r="B198" s="12"/>
       <c r="C198" s="20"/>
       <c r="D198" s="21"/>
-      <c r="E198" s="51"/>
+      <c r="E198" s="60"/>
       <c r="F198" s="47"/>
-      <c r="G198" s="51"/>
-      <c r="H198" s="54"/>
+      <c r="G198" s="60"/>
+      <c r="H198" s="63"/>
       <c r="I198" s="21"/>
       <c r="J198" s="21"/>
       <c r="K198" s="20"/>
@@ -7250,10 +7288,10 @@
       <c r="B199" s="12"/>
       <c r="C199" s="20"/>
       <c r="D199" s="21"/>
-      <c r="E199" s="51"/>
+      <c r="E199" s="60"/>
       <c r="F199" s="47"/>
-      <c r="G199" s="51"/>
-      <c r="H199" s="54"/>
+      <c r="G199" s="60"/>
+      <c r="H199" s="63"/>
       <c r="I199" s="21"/>
       <c r="J199" s="21"/>
       <c r="K199" s="20"/>
@@ -7280,10 +7318,10 @@
       <c r="B200" s="12"/>
       <c r="C200" s="20"/>
       <c r="D200" s="21"/>
-      <c r="E200" s="51"/>
+      <c r="E200" s="60"/>
       <c r="F200" s="47"/>
-      <c r="G200" s="51"/>
-      <c r="H200" s="54"/>
+      <c r="G200" s="60"/>
+      <c r="H200" s="63"/>
       <c r="I200" s="21"/>
       <c r="J200" s="21"/>
       <c r="K200" s="20"/>
@@ -7310,10 +7348,10 @@
       <c r="B201" s="12"/>
       <c r="C201" s="20"/>
       <c r="D201" s="21"/>
-      <c r="E201" s="51"/>
+      <c r="E201" s="60"/>
       <c r="F201" s="47"/>
-      <c r="G201" s="51"/>
-      <c r="H201" s="54"/>
+      <c r="G201" s="60"/>
+      <c r="H201" s="63"/>
       <c r="I201" s="21"/>
       <c r="J201" s="21"/>
       <c r="K201" s="20"/>
@@ -7340,10 +7378,10 @@
       <c r="B202" s="12"/>
       <c r="C202" s="20"/>
       <c r="D202" s="21"/>
-      <c r="E202" s="51"/>
+      <c r="E202" s="60"/>
       <c r="F202" s="47"/>
-      <c r="G202" s="51"/>
-      <c r="H202" s="54"/>
+      <c r="G202" s="60"/>
+      <c r="H202" s="63"/>
       <c r="I202" s="21"/>
       <c r="J202" s="21"/>
       <c r="K202" s="20"/>
@@ -7370,10 +7408,10 @@
       <c r="B203" s="12"/>
       <c r="C203" s="20"/>
       <c r="D203" s="21"/>
-      <c r="E203" s="51"/>
+      <c r="E203" s="60"/>
       <c r="F203" s="47"/>
-      <c r="G203" s="51"/>
-      <c r="H203" s="54"/>
+      <c r="G203" s="60"/>
+      <c r="H203" s="63"/>
       <c r="I203" s="21"/>
       <c r="J203" s="21"/>
       <c r="K203" s="20"/>
@@ -7400,10 +7438,10 @@
       <c r="B204" s="12"/>
       <c r="C204" s="20"/>
       <c r="D204" s="21"/>
-      <c r="E204" s="51"/>
+      <c r="E204" s="60"/>
       <c r="F204" s="47"/>
-      <c r="G204" s="51"/>
-      <c r="H204" s="54"/>
+      <c r="G204" s="60"/>
+      <c r="H204" s="63"/>
       <c r="I204" s="21"/>
       <c r="J204" s="21"/>
       <c r="K204" s="20"/>
@@ -7430,10 +7468,10 @@
       <c r="B205" s="12"/>
       <c r="C205" s="20"/>
       <c r="D205" s="21"/>
-      <c r="E205" s="51"/>
+      <c r="E205" s="60"/>
       <c r="F205" s="47"/>
-      <c r="G205" s="51"/>
-      <c r="H205" s="54"/>
+      <c r="G205" s="60"/>
+      <c r="H205" s="63"/>
       <c r="I205" s="21"/>
       <c r="J205" s="21"/>
       <c r="K205" s="20"/>

</xml_diff>

<commit_message>
Se marcan en el registro de usuarios, los datos obligatorios y se agrega componente Loading
</commit_message>
<xml_diff>
--- a/public/DownloadExcels/Mercancias.xlsx
+++ b/public/DownloadExcels/Mercancias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Mario\Desktop\Ecopcion Desarrollo\ecopFront-Desarrollo\public\DownloadExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97E6F78-7389-4B6B-A6D7-3A171E21EEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F08C241-BD8D-4ED2-A4E5-19348898F96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -824,15 +824,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -853,6 +844,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1127,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB689"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1147,24 +1147,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
@@ -1179,24 +1179,24 @@
       <c r="AB1" s="5"/>
     </row>
     <row r="2" spans="1:28" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
@@ -1211,24 +1211,24 @@
       <c r="AB2" s="5"/>
     </row>
     <row r="3" spans="1:28" ht="285" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
@@ -22362,13 +22362,13 @@
   <dimension ref="A1:K1001"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="67" customWidth="1"/>
     <col min="3" max="3" width="20" style="35" customWidth="1"/>
     <col min="4" max="4" width="20" style="37" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
@@ -22381,7 +22381,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="6" customFormat="1" ht="60.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="61" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="32" t="s">
@@ -22412,7 +22412,7 @@
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="62" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="33" t="s">
@@ -22442,7 +22442,7 @@
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="62" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="34">
@@ -22472,7 +22472,7 @@
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="62" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="34">
@@ -22502,7 +22502,7 @@
     </row>
     <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="62" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="34">
@@ -22529,7 +22529,7 @@
     </row>
     <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="63" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="52" t="s">
@@ -22547,7 +22547,7 @@
     </row>
     <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="63" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="52" t="s">
@@ -22565,7 +22565,7 @@
     </row>
     <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="63" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="25">
@@ -22581,7 +22581,7 @@
     </row>
     <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="64" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="25">
@@ -22596,7 +22596,7 @@
     </row>
     <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="65" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="25">
@@ -22608,7 +22608,7 @@
     </row>
     <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="66" t="s">
         <v>66</v>
       </c>
       <c r="F11" s="25">
@@ -22620,7 +22620,7 @@
     </row>
     <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="65" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="25">
@@ -22630,7 +22630,7 @@
     </row>
     <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="69" t="s">
+      <c r="B13" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F13" s="25">
@@ -22639,7 +22639,7 @@
     </row>
     <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="66" t="s">
         <v>68</v>
       </c>
       <c r="F14" s="25">
@@ -22648,7 +22648,7 @@
     </row>
     <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="65" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="25">
@@ -22657,7 +22657,7 @@
     </row>
     <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="65" t="s">
         <v>16</v>
       </c>
       <c r="F16" s="25">
@@ -22666,7 +22666,7 @@
     </row>
     <row r="17" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="65" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="25">
@@ -22675,7 +22675,7 @@
     </row>
     <row r="18" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="65" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="25">
@@ -22684,7 +22684,7 @@
     </row>
     <row r="19" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="65" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="25">
@@ -22693,7 +22693,7 @@
     </row>
     <row r="20" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="65" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="25">
@@ -22702,7 +22702,7 @@
     </row>
     <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="65" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="36"/>
@@ -22711,7 +22711,7 @@
     </row>
     <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="65" t="s">
         <v>22</v>
       </c>
       <c r="G22" s="46"/>
@@ -22719,7 +22719,7 @@
     </row>
     <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="63" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="46"/>
@@ -22727,7 +22727,7 @@
     </row>
     <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="63" t="s">
         <v>24</v>
       </c>
       <c r="G24" s="46"/>
@@ -22735,7 +22735,7 @@
     </row>
     <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="63" t="s">
         <v>25</v>
       </c>
       <c r="G25" s="46"/>
@@ -22743,7 +22743,7 @@
     </row>
     <row r="26" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="63" t="s">
         <v>26</v>
       </c>
       <c r="G26" s="46"/>
@@ -22751,7 +22751,7 @@
     </row>
     <row r="27" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="63" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="46"/>
@@ -22759,7 +22759,7 @@
     </row>
     <row r="28" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="66" t="s">
+      <c r="B28" s="63" t="s">
         <v>28</v>
       </c>
       <c r="G28" s="46"/>
@@ -22767,7 +22767,7 @@
     </row>
     <row r="29" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="63" t="s">
         <v>29</v>
       </c>
       <c r="G29" s="46"/>
@@ -22775,14 +22775,14 @@
     </row>
     <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="63" t="s">
         <v>30</v>
       </c>
       <c r="G30" s="46"/>
       <c r="H30" s="42"/>
     </row>
     <row r="31" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="66" t="s">
+      <c r="B31" s="63" t="s">
         <v>31</v>
       </c>
       <c r="G31" s="46"/>

</xml_diff>